<commit_message>
fix: update leaderboard scores
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/per-github/project-tennis/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0C13F0-8366-CB46-A4F3-FB8DD23ED7EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA38694-A5A8-DC43-9FA0-082B32AB9012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="37260" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33220" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -6916,8 +6916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I589"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="D419" sqref="D419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15442,7 +15442,7 @@
         <v>756</v>
       </c>
       <c r="D418" s="15">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="E418" s="1">
         <v>625</v>
@@ -18104,7 +18104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A46" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A46" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: Nam Tich name mobile + del Ty Long An
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/per-github/project-tennis/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277DF7FC-D98B-E54B-B964-757DB509FC6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD20A201-A463-8249-81CE-506A6D729560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25320" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="1142">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -2660,13 +2660,7 @@
     <t>Chuyển LV</t>
   </si>
   <si>
-    <t>Nam Tịnh</t>
-  </si>
-  <si>
     <t>Khang Trần</t>
-  </si>
-  <si>
-    <t>08185928855</t>
   </si>
   <si>
     <t>Hòa Nguyệt Quế</t>
@@ -5758,12 +5752,6 @@
     <t>0918008595</t>
   </si>
   <si>
-    <t>Tý Long An</t>
-  </si>
-  <si>
-    <t>0362029050</t>
-  </si>
-  <si>
     <t>Ben Q9</t>
   </si>
   <si>
@@ -6410,6 +6398,12 @@
   </si>
   <si>
     <t>Quốc Kỳ Hòa</t>
+  </si>
+  <si>
+    <t>Nam Tịch</t>
+  </si>
+  <si>
+    <t>0818592855</t>
   </si>
 </sst>
 </file>
@@ -6836,10 +6830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I642"/>
+  <dimension ref="A1:I641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A314" workbookViewId="0">
-      <selection activeCell="A324" sqref="A324:XFD324"/>
+    <sheetView tabSelected="1" topLeftCell="A443" workbookViewId="0">
+      <selection activeCell="F464" sqref="F464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7003,10 +6997,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D9" s="7">
         <v>685</v>
@@ -7020,10 +7014,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="D10" s="7">
         <v>600</v>
@@ -7116,7 +7110,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="D14" s="7">
         <v>650</v>
@@ -7140,7 +7134,7 @@
         <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="D15" s="5">
         <v>635</v>
@@ -7223,7 +7217,7 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D19" s="12">
         <v>635</v>
@@ -7247,7 +7241,7 @@
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D20" s="12">
         <v>640</v>
@@ -7271,7 +7265,7 @@
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="D21" s="12">
         <v>630</v>
@@ -7297,7 +7291,7 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D22" s="12">
         <v>635</v>
@@ -7318,10 +7312,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D23" s="12">
         <v>640</v>
@@ -7343,7 +7337,7 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D24" s="12">
         <v>650</v>
@@ -7387,7 +7381,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="D26" s="22">
         <v>640</v>
@@ -7476,7 +7470,7 @@
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="D30" s="12">
         <v>605</v>
@@ -7586,7 +7580,7 @@
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D35" s="12">
         <v>610</v>
@@ -7608,7 +7602,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>1058</v>
+        <v>1054</v>
       </c>
       <c r="D36" s="5">
         <v>605</v>
@@ -7629,7 +7623,7 @@
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D37" s="12">
         <v>665</v>
@@ -7649,7 +7643,7 @@
         <v>33</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="D38" s="7">
         <v>615</v>
@@ -7708,7 +7702,7 @@
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D41" s="12">
         <v>600</v>
@@ -7731,7 +7725,7 @@
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D42" s="12">
         <v>650</v>
@@ -7773,7 +7767,7 @@
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="D44" s="12">
         <v>630</v>
@@ -7994,7 +7988,7 @@
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D55" s="12">
         <v>625</v>
@@ -8015,7 +8009,7 @@
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="D56" s="12">
         <v>610</v>
@@ -8052,7 +8046,7 @@
         <v>53</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="D58" s="5">
         <v>650</v>
@@ -8067,7 +8061,7 @@
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D59" s="12">
         <v>600</v>
@@ -8108,10 +8102,10 @@
         <v>56</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="D61" s="12">
         <v>625</v>
@@ -8132,7 +8126,7 @@
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="11" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D62" s="12">
         <v>630</v>
@@ -8227,10 +8221,10 @@
         <v>62</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="D67" s="12">
         <v>615</v>
@@ -8267,10 +8261,10 @@
         <v>64</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="D69" s="12">
         <v>600</v>
@@ -8291,7 +8285,7 @@
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="11" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="D70" s="12">
         <v>605</v>
@@ -8418,7 +8412,7 @@
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D76" s="12">
         <v>660</v>
@@ -8502,7 +8496,7 @@
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="11" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="D80" s="12">
         <v>600</v>
@@ -8548,7 +8542,7 @@
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="11" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="D82" s="12">
         <v>670</v>
@@ -8592,7 +8586,7 @@
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="11" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="D84" s="12">
         <v>615</v>
@@ -8611,7 +8605,7 @@
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="11" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="D85" s="12">
         <v>635</v>
@@ -8630,7 +8624,7 @@
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="11" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="D86" s="12">
         <v>690</v>
@@ -8653,7 +8647,7 @@
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="11" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D87" s="12">
         <v>610</v>
@@ -8762,7 +8756,7 @@
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="D92" s="12">
         <v>655</v>
@@ -8782,10 +8776,10 @@
         <v>88</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="D93" s="12">
         <v>605</v>
@@ -8882,7 +8876,7 @@
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="11" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D98" s="12">
         <v>645</v>
@@ -9010,7 +9004,7 @@
       </c>
       <c r="B104" s="11"/>
       <c r="C104" s="11" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="D104" s="12">
         <v>630</v>
@@ -9054,7 +9048,7 @@
       </c>
       <c r="B106" s="11"/>
       <c r="C106" s="11" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D106" s="12">
         <v>660</v>
@@ -9074,7 +9068,7 @@
         <v>102</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="D107" s="7">
         <v>605</v>
@@ -9138,7 +9132,7 @@
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="11" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="D110" s="12">
         <v>600</v>
@@ -9157,7 +9151,7 @@
       </c>
       <c r="B111" s="11"/>
       <c r="C111" s="11" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D111" s="12">
         <v>625</v>
@@ -9235,7 +9229,7 @@
       </c>
       <c r="B115" s="11"/>
       <c r="C115" s="11" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="D115" s="12">
         <v>600</v>
@@ -9256,7 +9250,7 @@
       </c>
       <c r="B116" s="11"/>
       <c r="C116" s="11" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="D116" s="12">
         <v>675</v>
@@ -9296,7 +9290,7 @@
       </c>
       <c r="B118" s="11"/>
       <c r="C118" s="11" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="D118" s="12">
         <v>675</v>
@@ -9315,7 +9309,7 @@
       </c>
       <c r="B119" s="11"/>
       <c r="C119" s="11" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D119" s="12">
         <v>600</v>
@@ -9338,7 +9332,7 @@
       </c>
       <c r="B120" s="11"/>
       <c r="C120" s="11" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="D120" s="12">
         <v>600</v>
@@ -9382,7 +9376,7 @@
       </c>
       <c r="B122" s="11"/>
       <c r="C122" s="11" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D122" s="12">
         <v>645</v>
@@ -9405,7 +9399,7 @@
       </c>
       <c r="B123" s="11"/>
       <c r="C123" s="11" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="D123" s="12">
         <v>590</v>
@@ -9424,7 +9418,7 @@
       </c>
       <c r="B124" s="11"/>
       <c r="C124" s="11" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D124" s="12">
         <v>615</v>
@@ -9443,7 +9437,7 @@
       </c>
       <c r="B125" s="11"/>
       <c r="C125" s="11" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="D125" s="12">
         <v>635</v>
@@ -9505,7 +9499,7 @@
         <v>123</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>1056</v>
+        <v>1052</v>
       </c>
       <c r="D128" s="5">
         <v>635</v>
@@ -9523,7 +9517,7 @@
       </c>
       <c r="B129" s="11"/>
       <c r="C129" s="11" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D129" s="12">
         <v>610</v>
@@ -9561,7 +9555,7 @@
       </c>
       <c r="B131" s="11"/>
       <c r="C131" s="11" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D131" s="12">
         <v>680</v>
@@ -9580,7 +9574,7 @@
       </c>
       <c r="B132" s="11"/>
       <c r="C132" s="11" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D132" s="12">
         <v>590</v>
@@ -9622,7 +9616,7 @@
       </c>
       <c r="B134" s="11"/>
       <c r="C134" s="11" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D134" s="12">
         <v>635</v>
@@ -9760,7 +9754,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>1059</v>
+        <v>1055</v>
       </c>
       <c r="D141" s="7">
         <v>765</v>
@@ -9778,7 +9772,7 @@
       </c>
       <c r="B142" s="11"/>
       <c r="C142" s="11" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D142" s="12">
         <v>785</v>
@@ -9816,7 +9810,7 @@
       </c>
       <c r="B144" s="11"/>
       <c r="C144" s="11" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D144" s="12">
         <v>985</v>
@@ -9856,7 +9850,7 @@
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="11" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="D146" s="12">
         <v>850</v>
@@ -9894,7 +9888,7 @@
       </c>
       <c r="B148" s="11"/>
       <c r="C148" s="11" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D148" s="12">
         <v>790</v>
@@ -9912,7 +9906,7 @@
         <v>144</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="D149" s="7">
         <v>760</v>
@@ -9967,7 +9961,7 @@
       </c>
       <c r="B152" s="11"/>
       <c r="C152" s="11" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D152" s="12">
         <v>840</v>
@@ -9988,7 +9982,7 @@
       </c>
       <c r="B153" s="11"/>
       <c r="C153" s="11" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="D153" s="12">
         <v>785</v>
@@ -10007,7 +10001,7 @@
       </c>
       <c r="B154" s="11"/>
       <c r="C154" s="11" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D154" s="12">
         <v>880</v>
@@ -10047,7 +10041,7 @@
       </c>
       <c r="B156" s="11"/>
       <c r="C156" s="11" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D156" s="12">
         <v>830</v>
@@ -10068,7 +10062,7 @@
       </c>
       <c r="B157" s="11"/>
       <c r="C157" s="11" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D157" s="12">
         <v>935</v>
@@ -10127,7 +10121,7 @@
       </c>
       <c r="B160" s="11"/>
       <c r="C160" s="11" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="D160" s="12">
         <v>920</v>
@@ -10186,7 +10180,7 @@
       </c>
       <c r="B163" s="11"/>
       <c r="C163" s="11" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D163" s="12">
         <v>810</v>
@@ -10207,7 +10201,7 @@
       </c>
       <c r="B164" s="11"/>
       <c r="C164" s="11" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D164" s="12">
         <v>755</v>
@@ -10228,7 +10222,7 @@
       </c>
       <c r="B165" s="11"/>
       <c r="C165" s="11" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D165" s="12">
         <v>605</v>
@@ -10247,7 +10241,7 @@
       </c>
       <c r="B166" s="11"/>
       <c r="C166" s="11" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D166" s="12">
         <v>990</v>
@@ -10286,7 +10280,7 @@
         <v>163</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D168" s="7">
         <v>735</v>
@@ -10304,7 +10298,7 @@
       </c>
       <c r="B169" s="11"/>
       <c r="C169" s="11" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D169" s="12">
         <v>630</v>
@@ -10346,7 +10340,7 @@
       </c>
       <c r="B171" s="11"/>
       <c r="C171" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D171" s="12">
         <v>750</v>
@@ -10428,7 +10422,7 @@
       </c>
       <c r="B175" s="11"/>
       <c r="C175" s="11" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="D175" s="12">
         <v>910</v>
@@ -10468,7 +10462,7 @@
       </c>
       <c r="B177" s="11"/>
       <c r="C177" s="11" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D177" s="12">
         <v>930</v>
@@ -10489,7 +10483,7 @@
       </c>
       <c r="B178" s="11"/>
       <c r="C178" s="11" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D178" s="12">
         <v>955</v>
@@ -10510,7 +10504,7 @@
       </c>
       <c r="B179" s="11"/>
       <c r="C179" s="11" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D179" s="12">
         <v>1010</v>
@@ -10531,7 +10525,7 @@
       </c>
       <c r="B180" s="11"/>
       <c r="C180" s="11" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="D180" s="12">
         <v>670</v>
@@ -10571,7 +10565,7 @@
       </c>
       <c r="B182" s="11"/>
       <c r="C182" s="11" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D182" s="12">
         <v>890</v>
@@ -10590,7 +10584,7 @@
       </c>
       <c r="B183" s="11"/>
       <c r="C183" s="11" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="D183" s="12">
         <v>815</v>
@@ -10609,7 +10603,7 @@
       </c>
       <c r="B184" s="11"/>
       <c r="C184" s="11" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D184" s="12">
         <v>835</v>
@@ -10630,7 +10624,7 @@
       </c>
       <c r="B185" s="11"/>
       <c r="C185" s="11" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="D185" s="12">
         <v>735</v>
@@ -10651,7 +10645,7 @@
       </c>
       <c r="B186" s="11"/>
       <c r="C186" s="11" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D186" s="12">
         <v>780</v>
@@ -10670,7 +10664,7 @@
       </c>
       <c r="B187" s="11"/>
       <c r="C187" s="11" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="D187" s="12">
         <v>810</v>
@@ -10689,7 +10683,7 @@
       </c>
       <c r="B188" s="11"/>
       <c r="C188" s="11" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D188" s="12">
         <v>880</v>
@@ -10710,7 +10704,7 @@
       </c>
       <c r="B189" s="11"/>
       <c r="C189" s="11" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D189" s="12">
         <v>885</v>
@@ -10730,7 +10724,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="D190" s="7">
         <v>695</v>
@@ -10764,7 +10758,7 @@
       </c>
       <c r="B192" s="11"/>
       <c r="C192" s="11" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D192" s="12">
         <v>880</v>
@@ -10785,7 +10779,7 @@
       </c>
       <c r="B193" s="11"/>
       <c r="C193" s="11" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D193" s="12">
         <v>745</v>
@@ -10844,7 +10838,7 @@
       </c>
       <c r="B196" s="11"/>
       <c r="C196" s="11" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D196" s="12">
         <v>790</v>
@@ -10880,7 +10874,7 @@
       </c>
       <c r="B198" s="11"/>
       <c r="C198" s="11" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="D198" s="12">
         <v>740</v>
@@ -10899,7 +10893,7 @@
       </c>
       <c r="B199" s="11"/>
       <c r="C199" s="11" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D199" s="12">
         <v>730</v>
@@ -10918,7 +10912,7 @@
       </c>
       <c r="B200" s="11"/>
       <c r="C200" s="11" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="D200" s="12">
         <v>745</v>
@@ -10951,7 +10945,7 @@
       </c>
       <c r="B202" s="11"/>
       <c r="C202" s="11" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D202" s="12">
         <v>660</v>
@@ -11028,7 +11022,7 @@
         <v>201</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="D206" s="7">
         <v>690</v>
@@ -11062,7 +11056,7 @@
       </c>
       <c r="B208" s="11"/>
       <c r="C208" s="11" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D208" s="12">
         <v>760</v>
@@ -11081,7 +11075,7 @@
       </c>
       <c r="B209" s="11"/>
       <c r="C209" s="11" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D209" s="12">
         <v>725</v>
@@ -13822,7 +13816,7 @@
       </c>
       <c r="B341" s="11"/>
       <c r="C341" s="11" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D341" s="12">
         <v>800</v>
@@ -15490,7 +15484,7 @@
       </c>
       <c r="F423" s="11"/>
       <c r="G423" s="11" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="H423" s="11"/>
       <c r="I423" s="11"/>
@@ -15648,7 +15642,7 @@
         <v>595</v>
       </c>
       <c r="F431" s="10" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
     </row>
     <row r="432" spans="1:9" x14ac:dyDescent="0.2">
@@ -16078,7 +16072,7 @@
       </c>
       <c r="B453" s="11"/>
       <c r="C453" s="11" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="D453" s="12">
         <v>645</v>
@@ -16196,7 +16190,7 @@
         <v>718</v>
       </c>
       <c r="C459" s="11" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D459" s="12">
         <v>640</v>
@@ -16272,7 +16266,7 @@
       </c>
       <c r="B463" s="11"/>
       <c r="C463" s="11" t="s">
-        <v>722</v>
+        <v>1140</v>
       </c>
       <c r="D463" s="12">
         <v>615</v>
@@ -16281,7 +16275,7 @@
         <v>615</v>
       </c>
       <c r="F463" s="16" t="s">
-        <v>724</v>
+        <v>1141</v>
       </c>
       <c r="G463" s="11"/>
       <c r="H463" s="11"/>
@@ -16292,7 +16286,7 @@
         <v>460</v>
       </c>
       <c r="C464" s="6" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D464" s="7">
         <v>640</v>
@@ -16307,7 +16301,7 @@
       </c>
       <c r="B465" s="11"/>
       <c r="C465" s="11" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D465" s="12">
         <v>630</v>
@@ -16316,7 +16310,7 @@
         <v>625</v>
       </c>
       <c r="F465" s="16" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="G465" s="11"/>
       <c r="H465" s="11"/>
@@ -16328,7 +16322,7 @@
       </c>
       <c r="B466" s="11"/>
       <c r="C466" s="11" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="D466" s="12">
         <v>615</v>
@@ -16337,7 +16331,7 @@
         <v>615</v>
       </c>
       <c r="F466" s="16" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="G466" s="11"/>
       <c r="H466" s="11"/>
@@ -16349,7 +16343,7 @@
       </c>
       <c r="B467" s="11"/>
       <c r="C467" s="11" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="D467" s="12">
         <v>600</v>
@@ -16368,7 +16362,7 @@
       </c>
       <c r="B468" s="11"/>
       <c r="C468" s="11" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="D468" s="12">
         <v>645</v>
@@ -16377,7 +16371,7 @@
         <v>640</v>
       </c>
       <c r="F468" s="16" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="G468" s="11"/>
       <c r="H468" s="11"/>
@@ -16389,7 +16383,7 @@
       </c>
       <c r="B469" s="11"/>
       <c r="C469" s="11" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="D469" s="12">
         <v>585</v>
@@ -16408,7 +16402,7 @@
       </c>
       <c r="B470" s="11"/>
       <c r="C470" s="11" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="D470" s="12">
         <v>620</v>
@@ -16427,7 +16421,7 @@
       </c>
       <c r="B471" s="11"/>
       <c r="C471" s="11" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D471" s="12">
         <v>640</v>
@@ -16446,7 +16440,7 @@
       </c>
       <c r="B472" s="11"/>
       <c r="C472" s="11" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D472" s="12">
         <v>610</v>
@@ -16465,7 +16459,7 @@
       </c>
       <c r="B473" s="11"/>
       <c r="C473" s="11" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D473" s="12">
         <v>630</v>
@@ -16484,7 +16478,7 @@
       </c>
       <c r="B474" s="11"/>
       <c r="C474" s="11" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D474" s="12">
         <v>590</v>
@@ -16503,7 +16497,7 @@
       </c>
       <c r="B475" s="11"/>
       <c r="C475" s="11" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D475" s="12">
         <v>615</v>
@@ -16522,7 +16516,7 @@
       </c>
       <c r="B476" s="11"/>
       <c r="C476" s="11" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D476" s="12">
         <v>630</v>
@@ -16541,7 +16535,7 @@
       </c>
       <c r="B477" s="11"/>
       <c r="C477" s="11" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D477" s="12">
         <v>630</v>
@@ -16550,7 +16544,7 @@
         <v>625</v>
       </c>
       <c r="F477" s="16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G477" s="11"/>
       <c r="H477" s="11"/>
@@ -16562,7 +16556,7 @@
       </c>
       <c r="B478" s="11"/>
       <c r="C478" s="11" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D478" s="12">
         <v>620</v>
@@ -16581,7 +16575,7 @@
       </c>
       <c r="B479" s="11"/>
       <c r="C479" s="11" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D479" s="12">
         <v>610</v>
@@ -16600,7 +16594,7 @@
       </c>
       <c r="B480" s="11"/>
       <c r="C480" s="11" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D480" s="12">
         <v>655</v>
@@ -16609,7 +16603,7 @@
         <v>645</v>
       </c>
       <c r="F480" s="16" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G480" s="11"/>
       <c r="H480" s="11"/>
@@ -16621,7 +16615,7 @@
       </c>
       <c r="B481" s="11"/>
       <c r="C481" s="11" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D481" s="12">
         <v>605</v>
@@ -16640,7 +16634,7 @@
       </c>
       <c r="B482" s="11"/>
       <c r="C482" s="11" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D482" s="12">
         <v>620</v>
@@ -16659,7 +16653,7 @@
       </c>
       <c r="B483" s="11"/>
       <c r="C483" s="11" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D483" s="12">
         <v>615</v>
@@ -16678,7 +16672,7 @@
       </c>
       <c r="B484" s="11"/>
       <c r="C484" s="11" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="D484" s="12">
         <v>635</v>
@@ -16697,7 +16691,7 @@
       </c>
       <c r="B485" s="11"/>
       <c r="C485" s="11" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D485" s="12">
         <v>620</v>
@@ -16716,7 +16710,7 @@
       </c>
       <c r="B486" s="11"/>
       <c r="C486" s="11" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D486" s="12">
         <v>615</v>
@@ -16725,7 +16719,7 @@
         <v>610</v>
       </c>
       <c r="F486" s="16" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="G486" s="11"/>
       <c r="H486" s="11"/>
@@ -16737,7 +16731,7 @@
       </c>
       <c r="B487" s="11"/>
       <c r="C487" s="11" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D487" s="12">
         <v>625</v>
@@ -16746,7 +16740,7 @@
         <v>620</v>
       </c>
       <c r="F487" s="16" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="G487" s="11"/>
       <c r="H487" s="11"/>
@@ -16758,7 +16752,7 @@
       </c>
       <c r="B488" s="11"/>
       <c r="C488" s="11" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="D488" s="12">
         <v>610</v>
@@ -16767,7 +16761,7 @@
         <v>610</v>
       </c>
       <c r="F488" s="16" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G488" s="11"/>
       <c r="H488" s="11"/>
@@ -16779,7 +16773,7 @@
       </c>
       <c r="B489" s="11"/>
       <c r="C489" s="11" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="D489" s="12">
         <v>630</v>
@@ -16798,7 +16792,7 @@
       </c>
       <c r="B490" s="11"/>
       <c r="C490" s="11" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="D490" s="12">
         <v>630</v>
@@ -16807,7 +16801,7 @@
         <v>625</v>
       </c>
       <c r="F490" s="16" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="G490" s="11"/>
       <c r="H490" s="11"/>
@@ -16819,7 +16813,7 @@
       </c>
       <c r="B491" s="11"/>
       <c r="C491" s="11" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="D491" s="12">
         <v>585</v>
@@ -16838,7 +16832,7 @@
       </c>
       <c r="B492" s="11"/>
       <c r="C492" s="11" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="D492" s="12">
         <v>610</v>
@@ -16857,7 +16851,7 @@
       </c>
       <c r="B493" s="11"/>
       <c r="C493" s="11" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="D493" s="12">
         <v>590</v>
@@ -16876,7 +16870,7 @@
       </c>
       <c r="B494" s="11"/>
       <c r="C494" s="11" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="D494" s="12">
         <v>670</v>
@@ -16895,7 +16889,7 @@
       </c>
       <c r="B495" s="11"/>
       <c r="C495" s="11" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="D495" s="12">
         <v>635</v>
@@ -16913,7 +16907,7 @@
         <v>492</v>
       </c>
       <c r="C496" s="4" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="D496" s="5">
         <v>645</v>
@@ -16928,7 +16922,7 @@
       </c>
       <c r="B497" s="11"/>
       <c r="C497" s="11" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="D497" s="12">
         <v>605</v>
@@ -16937,7 +16931,7 @@
         <v>605</v>
       </c>
       <c r="F497" s="16" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="G497" s="11"/>
       <c r="H497" s="11"/>
@@ -16949,7 +16943,7 @@
       </c>
       <c r="B498" s="11"/>
       <c r="C498" s="11" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="D498" s="12">
         <v>640</v>
@@ -16968,7 +16962,7 @@
       </c>
       <c r="B499" s="11"/>
       <c r="C499" s="11" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="D499" s="12">
         <v>610</v>
@@ -16987,7 +16981,7 @@
       </c>
       <c r="B500" s="11"/>
       <c r="C500" s="11" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="D500" s="12">
         <v>650</v>
@@ -17006,7 +17000,7 @@
       </c>
       <c r="B501" s="11"/>
       <c r="C501" s="11" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="D501" s="12">
         <v>600</v>
@@ -17025,7 +17019,7 @@
       </c>
       <c r="B502" s="11"/>
       <c r="C502" s="11" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="D502" s="12">
         <v>650</v>
@@ -17044,7 +17038,7 @@
       </c>
       <c r="B503" s="11"/>
       <c r="C503" s="11" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="D503" s="12">
         <v>640</v>
@@ -17053,7 +17047,7 @@
         <v>635</v>
       </c>
       <c r="F503" s="16" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G503" s="11"/>
       <c r="H503" s="11"/>
@@ -17065,7 +17059,7 @@
       </c>
       <c r="B504" s="11"/>
       <c r="C504" s="11" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="D504" s="12">
         <v>625</v>
@@ -17084,7 +17078,7 @@
       </c>
       <c r="B505" s="11"/>
       <c r="C505" s="11" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="D505" s="12">
         <v>610</v>
@@ -17103,7 +17097,7 @@
       </c>
       <c r="B506" s="11"/>
       <c r="C506" s="11" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="D506" s="12">
         <v>640</v>
@@ -17122,7 +17116,7 @@
       </c>
       <c r="B507" s="11"/>
       <c r="C507" s="11" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="D507" s="12">
         <v>610</v>
@@ -17131,7 +17125,7 @@
         <v>610</v>
       </c>
       <c r="F507" s="16" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="G507" s="11"/>
       <c r="H507" s="11"/>
@@ -17143,7 +17137,7 @@
       </c>
       <c r="B508" s="11"/>
       <c r="C508" s="11" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="D508" s="12">
         <v>660</v>
@@ -17152,7 +17146,7 @@
         <v>655</v>
       </c>
       <c r="F508" s="16" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G508" s="11"/>
       <c r="H508" s="11"/>
@@ -17164,7 +17158,7 @@
       </c>
       <c r="B509" s="11"/>
       <c r="C509" s="11" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D509" s="12">
         <v>655</v>
@@ -17173,7 +17167,7 @@
         <v>645</v>
       </c>
       <c r="F509" s="16" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="G509" s="11"/>
       <c r="H509" s="11"/>
@@ -17185,7 +17179,7 @@
       </c>
       <c r="B510" s="11"/>
       <c r="C510" s="11" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="D510" s="12">
         <v>625</v>
@@ -17204,7 +17198,7 @@
       </c>
       <c r="B511" s="11"/>
       <c r="C511" s="11" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="D511" s="12">
         <v>605</v>
@@ -17213,7 +17207,7 @@
         <v>605</v>
       </c>
       <c r="F511" s="16" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="G511" s="11"/>
       <c r="H511" s="11"/>
@@ -17225,7 +17219,7 @@
       </c>
       <c r="B512" s="11"/>
       <c r="C512" s="11" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="D512" s="12">
         <v>650</v>
@@ -17234,7 +17228,7 @@
         <v>640</v>
       </c>
       <c r="F512" s="16" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="G512" s="11"/>
       <c r="H512" s="11"/>
@@ -17246,7 +17240,7 @@
       </c>
       <c r="B513" s="11"/>
       <c r="C513" s="11" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="D513" s="12">
         <v>640</v>
@@ -17255,7 +17249,7 @@
         <v>635</v>
       </c>
       <c r="F513" s="16" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G513" s="11"/>
       <c r="H513" s="11"/>
@@ -17267,7 +17261,7 @@
       </c>
       <c r="B514" s="11"/>
       <c r="C514" s="11" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="D514" s="12">
         <v>585</v>
@@ -17276,7 +17270,7 @@
         <v>585</v>
       </c>
       <c r="F514" s="16" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="G514" s="11"/>
       <c r="H514" s="11"/>
@@ -17288,7 +17282,7 @@
       </c>
       <c r="B515" s="11"/>
       <c r="C515" s="11" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="D515" s="12">
         <v>640</v>
@@ -17307,7 +17301,7 @@
       </c>
       <c r="B516" s="11"/>
       <c r="C516" s="11" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="D516" s="12">
         <v>625</v>
@@ -17316,7 +17310,7 @@
         <v>615</v>
       </c>
       <c r="F516" s="16" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G516" s="11"/>
       <c r="H516" s="11"/>
@@ -17328,7 +17322,7 @@
       </c>
       <c r="B517" s="11"/>
       <c r="C517" s="11" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="D517" s="12">
         <v>625</v>
@@ -17337,7 +17331,7 @@
         <v>615</v>
       </c>
       <c r="F517" s="16" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="G517" s="11"/>
       <c r="H517" s="11"/>
@@ -17349,7 +17343,7 @@
       </c>
       <c r="B518" s="11"/>
       <c r="C518" s="11" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="D518" s="12">
         <v>600</v>
@@ -17358,7 +17352,7 @@
         <v>600</v>
       </c>
       <c r="F518" s="16" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G518" s="11"/>
       <c r="H518" s="11"/>
@@ -17370,7 +17364,7 @@
       </c>
       <c r="B519" s="11"/>
       <c r="C519" s="11" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="D519" s="12">
         <v>670</v>
@@ -17379,7 +17373,7 @@
         <v>660</v>
       </c>
       <c r="F519" s="16" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G519" s="11"/>
       <c r="H519" s="11"/>
@@ -17390,7 +17384,7 @@
         <v>516</v>
       </c>
       <c r="C520" s="6" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="D520" s="7">
         <v>580</v>
@@ -17404,7 +17398,7 @@
         <v>517</v>
       </c>
       <c r="C521" s="6" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="D521" s="7">
         <v>660</v>
@@ -17413,7 +17407,7 @@
         <v>650</v>
       </c>
       <c r="F521" s="8" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="522" spans="1:9" x14ac:dyDescent="0.2">
@@ -17422,7 +17416,7 @@
       </c>
       <c r="B522" s="11"/>
       <c r="C522" s="11" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D522" s="12">
         <v>590</v>
@@ -17431,7 +17425,7 @@
         <v>590</v>
       </c>
       <c r="F522" s="16" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="G522" s="11"/>
       <c r="H522" s="11"/>
@@ -17443,7 +17437,7 @@
       </c>
       <c r="B523" s="11"/>
       <c r="C523" s="11" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="D523" s="12">
         <v>650</v>
@@ -17452,7 +17446,7 @@
         <v>640</v>
       </c>
       <c r="F523" s="16" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="G523" s="11"/>
       <c r="H523" s="11"/>
@@ -17464,7 +17458,7 @@
       </c>
       <c r="B524" s="11"/>
       <c r="C524" s="11" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="D524" s="12">
         <v>610</v>
@@ -17473,7 +17467,7 @@
         <v>610</v>
       </c>
       <c r="F524" s="16" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="G524" s="11"/>
       <c r="H524" s="11"/>
@@ -17485,7 +17479,7 @@
       </c>
       <c r="B525" s="11"/>
       <c r="C525" s="11" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="D525" s="12">
         <v>670</v>
@@ -17494,7 +17488,7 @@
         <v>660</v>
       </c>
       <c r="F525" s="16" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G525" s="11"/>
       <c r="H525" s="11"/>
@@ -17506,7 +17500,7 @@
       </c>
       <c r="B526" s="11"/>
       <c r="C526" s="11" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="D526" s="12">
         <v>620</v>
@@ -17515,7 +17509,7 @@
         <v>610</v>
       </c>
       <c r="F526" s="16" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="G526" s="11"/>
       <c r="H526" s="11"/>
@@ -17527,7 +17521,7 @@
       </c>
       <c r="B527" s="11"/>
       <c r="C527" s="11" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="D527" s="12">
         <v>635</v>
@@ -17536,7 +17530,7 @@
         <v>625</v>
       </c>
       <c r="F527" s="16" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="G527" s="11"/>
       <c r="H527" s="11"/>
@@ -17548,7 +17542,7 @@
       </c>
       <c r="B528" s="11"/>
       <c r="C528" s="11" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="D528" s="12">
         <v>710</v>
@@ -17557,7 +17551,7 @@
         <v>700</v>
       </c>
       <c r="F528" s="16" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="G528" s="11"/>
       <c r="H528" s="11"/>
@@ -17569,7 +17563,7 @@
       </c>
       <c r="B529" s="11"/>
       <c r="C529" s="11" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="D529" s="12">
         <v>610</v>
@@ -17588,7 +17582,7 @@
       </c>
       <c r="B530" s="11"/>
       <c r="C530" s="11" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="D530" s="12">
         <v>710</v>
@@ -17597,7 +17591,7 @@
         <v>700</v>
       </c>
       <c r="F530" s="16" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="G530" s="11"/>
       <c r="H530" s="11"/>
@@ -17609,7 +17603,7 @@
       </c>
       <c r="B531" s="11"/>
       <c r="C531" s="11" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D531" s="12">
         <v>630</v>
@@ -17618,7 +17612,7 @@
         <v>620</v>
       </c>
       <c r="F531" s="16" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G531" s="11"/>
       <c r="H531" s="11"/>
@@ -17630,7 +17624,7 @@
       </c>
       <c r="B532" s="11"/>
       <c r="C532" s="11" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="D532" s="12">
         <v>670</v>
@@ -17649,7 +17643,7 @@
       </c>
       <c r="B533" s="11"/>
       <c r="C533" s="11" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="D533" s="12">
         <v>775</v>
@@ -17668,7 +17662,7 @@
       </c>
       <c r="B534" s="11"/>
       <c r="C534" s="11" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="D534" s="12">
         <v>630</v>
@@ -17687,7 +17681,7 @@
       </c>
       <c r="B535" s="11"/>
       <c r="C535" s="11" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D535" s="12">
         <v>760</v>
@@ -17706,7 +17700,7 @@
       </c>
       <c r="B536" s="11"/>
       <c r="C536" s="11" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D536" s="12">
         <v>740</v>
@@ -17715,7 +17709,7 @@
         <v>735</v>
       </c>
       <c r="F536" s="16" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="G536" s="11"/>
       <c r="H536" s="11"/>
@@ -17727,7 +17721,7 @@
       </c>
       <c r="B537" s="11"/>
       <c r="C537" s="11" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D537" s="12">
         <v>640</v>
@@ -17746,7 +17740,7 @@
       </c>
       <c r="B538" s="11"/>
       <c r="C538" s="11" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D538" s="12">
         <v>700</v>
@@ -17765,7 +17759,7 @@
       </c>
       <c r="B539" s="11"/>
       <c r="C539" s="11" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="D539" s="12">
         <v>720</v>
@@ -17786,7 +17780,7 @@
       </c>
       <c r="B540" s="11"/>
       <c r="C540" s="11" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="D540" s="12">
         <v>720</v>
@@ -17795,7 +17789,7 @@
         <v>710</v>
       </c>
       <c r="F540" s="16" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="G540" s="11"/>
       <c r="H540" s="11"/>
@@ -17807,7 +17801,7 @@
       </c>
       <c r="B541" s="11"/>
       <c r="C541" s="11" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="D541" s="12">
         <v>640</v>
@@ -17816,7 +17810,7 @@
         <v>630</v>
       </c>
       <c r="F541" s="16" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="G541" s="11"/>
       <c r="H541" s="11"/>
@@ -17828,7 +17822,7 @@
       </c>
       <c r="B542" s="11"/>
       <c r="C542" s="11" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="D542" s="12">
         <v>730</v>
@@ -17847,7 +17841,7 @@
       </c>
       <c r="B543" s="11"/>
       <c r="C543" s="11" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="D543" s="12">
         <v>625</v>
@@ -17866,7 +17860,7 @@
       </c>
       <c r="B544" s="11"/>
       <c r="C544" s="11" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="D544" s="12">
         <v>690</v>
@@ -17875,7 +17869,7 @@
         <v>680</v>
       </c>
       <c r="F544" s="16" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="G544" s="11"/>
       <c r="H544" s="11"/>
@@ -17887,7 +17881,7 @@
       </c>
       <c r="B545" s="11"/>
       <c r="C545" s="11" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="D545" s="12">
         <v>630</v>
@@ -17906,7 +17900,7 @@
       </c>
       <c r="B546" s="11"/>
       <c r="C546" s="11" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="D546" s="12">
         <v>725</v>
@@ -17925,7 +17919,7 @@
       </c>
       <c r="B547" s="11"/>
       <c r="C547" s="11" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="D547" s="12">
         <v>670</v>
@@ -17944,7 +17938,7 @@
       </c>
       <c r="B548" s="11"/>
       <c r="C548" s="11" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="D548" s="12">
         <v>670</v>
@@ -17963,7 +17957,7 @@
       </c>
       <c r="B549" s="11"/>
       <c r="C549" s="11" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="D549" s="12">
         <v>725</v>
@@ -17982,7 +17976,7 @@
       </c>
       <c r="B550" s="11"/>
       <c r="C550" s="11" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="D550" s="12">
         <v>625</v>
@@ -17991,7 +17985,7 @@
         <v>615</v>
       </c>
       <c r="F550" s="16" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="G550" s="11"/>
       <c r="H550" s="11"/>
@@ -18003,7 +17997,7 @@
       </c>
       <c r="B551" s="11"/>
       <c r="C551" s="11" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="D551" s="12">
         <v>630</v>
@@ -18022,7 +18016,7 @@
       </c>
       <c r="B552" s="11"/>
       <c r="C552" s="11" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="D552" s="12">
         <v>690</v>
@@ -18031,7 +18025,7 @@
         <v>675</v>
       </c>
       <c r="F552" s="16" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="G552" s="11"/>
       <c r="H552" s="11"/>
@@ -18043,7 +18037,7 @@
       </c>
       <c r="B553" s="11"/>
       <c r="C553" s="11" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D553" s="12">
         <v>700</v>
@@ -18052,7 +18046,7 @@
         <v>690</v>
       </c>
       <c r="F553" s="16" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="G553" s="11"/>
       <c r="H553" s="11"/>
@@ -18064,7 +18058,7 @@
       </c>
       <c r="B554" s="11"/>
       <c r="C554" s="11" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="D554" s="12">
         <v>630</v>
@@ -18083,7 +18077,7 @@
       </c>
       <c r="B555" s="11"/>
       <c r="C555" s="11" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="D555" s="12">
         <v>660</v>
@@ -18092,7 +18086,7 @@
         <v>650</v>
       </c>
       <c r="F555" s="16" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="G555" s="11"/>
       <c r="H555" s="11"/>
@@ -18104,7 +18098,7 @@
       </c>
       <c r="B556" s="11"/>
       <c r="C556" s="11" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="D556" s="12">
         <v>620</v>
@@ -18123,7 +18117,7 @@
       </c>
       <c r="B557" s="11"/>
       <c r="C557" s="11" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="D557" s="12">
         <v>650</v>
@@ -18132,7 +18126,7 @@
         <v>645</v>
       </c>
       <c r="F557" s="16" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="G557" s="11"/>
       <c r="H557" s="11"/>
@@ -18144,7 +18138,7 @@
       </c>
       <c r="B558" s="11"/>
       <c r="C558" s="11" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D558" s="12">
         <v>625</v>
@@ -18153,7 +18147,7 @@
         <v>620</v>
       </c>
       <c r="F558" s="16" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="G558" s="11"/>
       <c r="H558" s="11"/>
@@ -18164,7 +18158,7 @@
         <v>555</v>
       </c>
       <c r="C559" s="6" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="D559" s="7">
         <v>580</v>
@@ -18178,7 +18172,7 @@
         <v>556</v>
       </c>
       <c r="C560" s="6" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="D560" s="7">
         <v>620</v>
@@ -18187,7 +18181,7 @@
         <v>615</v>
       </c>
       <c r="F560" s="8" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="561" spans="1:9" x14ac:dyDescent="0.2">
@@ -18196,7 +18190,7 @@
       </c>
       <c r="B561" s="11"/>
       <c r="C561" s="11" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="D561" s="12">
         <v>775</v>
@@ -18215,7 +18209,7 @@
       </c>
       <c r="B562" s="11"/>
       <c r="C562" s="11" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="D562" s="12">
         <v>635</v>
@@ -18224,7 +18218,7 @@
         <v>630</v>
       </c>
       <c r="F562" s="16" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="G562" s="11"/>
       <c r="H562" s="11"/>
@@ -18236,7 +18230,7 @@
       </c>
       <c r="B563" s="11"/>
       <c r="C563" s="11" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="D563" s="12">
         <v>610</v>
@@ -18255,7 +18249,7 @@
       </c>
       <c r="B564" s="11"/>
       <c r="C564" s="11" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="D564" s="12">
         <v>640</v>
@@ -18274,7 +18268,7 @@
       </c>
       <c r="B565" s="11"/>
       <c r="C565" s="11" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="D565" s="12">
         <v>650</v>
@@ -18292,7 +18286,7 @@
         <v>562</v>
       </c>
       <c r="C566" s="4" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="D566" s="5">
         <v>670</v>
@@ -18307,7 +18301,7 @@
       </c>
       <c r="B567" s="11"/>
       <c r="C567" s="11" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="D567" s="12">
         <v>635</v>
@@ -18316,7 +18310,7 @@
         <v>625</v>
       </c>
       <c r="F567" s="16" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="G567" s="11"/>
       <c r="H567" s="11"/>
@@ -18328,7 +18322,7 @@
       </c>
       <c r="B568" s="11"/>
       <c r="C568" s="11" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="D568" s="12">
         <v>600</v>
@@ -18347,7 +18341,7 @@
       </c>
       <c r="B569" s="11"/>
       <c r="C569" s="11" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="D569" s="12">
         <v>645</v>
@@ -18356,7 +18350,7 @@
         <v>640</v>
       </c>
       <c r="F569" s="16" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="G569" s="11"/>
       <c r="H569" s="11"/>
@@ -18368,7 +18362,7 @@
       </c>
       <c r="B570" s="11"/>
       <c r="C570" s="11" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D570" s="12">
         <v>630</v>
@@ -18377,7 +18371,7 @@
         <v>625</v>
       </c>
       <c r="F570" s="16" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="G570" s="11"/>
       <c r="H570" s="11"/>
@@ -18389,7 +18383,7 @@
       </c>
       <c r="B571" s="11"/>
       <c r="C571" s="11" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="D571" s="12">
         <v>660</v>
@@ -18398,7 +18392,7 @@
         <v>650</v>
       </c>
       <c r="F571" s="16" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="G571" s="11"/>
       <c r="H571" s="11"/>
@@ -18410,7 +18404,7 @@
       </c>
       <c r="B572" s="11"/>
       <c r="C572" s="11" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="D572" s="12">
         <v>640</v>
@@ -18419,7 +18413,7 @@
         <v>635</v>
       </c>
       <c r="F572" s="16" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="G572" s="11"/>
       <c r="H572" s="11"/>
@@ -18431,7 +18425,7 @@
       </c>
       <c r="B573" s="11"/>
       <c r="C573" s="11" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="D573" s="12">
         <v>690</v>
@@ -18440,7 +18434,7 @@
         <v>680</v>
       </c>
       <c r="F573" s="16" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="G573" s="11"/>
       <c r="H573" s="11"/>
@@ -18452,7 +18446,7 @@
       </c>
       <c r="B574" s="11"/>
       <c r="C574" s="11" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="D574" s="12">
         <v>640</v>
@@ -18471,7 +18465,7 @@
       </c>
       <c r="B575" s="11"/>
       <c r="C575" s="11" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="D575" s="12">
         <v>645</v>
@@ -18480,7 +18474,7 @@
         <v>640</v>
       </c>
       <c r="F575" s="16" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="G575" s="11"/>
       <c r="H575" s="11"/>
@@ -18492,7 +18486,7 @@
       </c>
       <c r="B576" s="11"/>
       <c r="C576" s="11" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="D576" s="12">
         <v>650</v>
@@ -18501,7 +18495,7 @@
         <v>640</v>
       </c>
       <c r="F576" s="16" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="G576" s="11"/>
       <c r="H576" s="11"/>
@@ -18513,7 +18507,7 @@
       </c>
       <c r="B577" s="11"/>
       <c r="C577" s="11" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="D577" s="12">
         <v>690</v>
@@ -18532,7 +18526,7 @@
       </c>
       <c r="B578" s="11"/>
       <c r="C578" s="11" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="D578" s="12">
         <v>675</v>
@@ -18541,7 +18535,7 @@
         <v>665</v>
       </c>
       <c r="F578" s="16" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G578" s="11"/>
       <c r="H578" s="11"/>
@@ -18552,7 +18546,7 @@
         <v>575</v>
       </c>
       <c r="C579" s="6" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D579" s="7">
         <v>585</v>
@@ -18567,7 +18561,7 @@
       </c>
       <c r="B580" s="11"/>
       <c r="C580" s="11" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D580" s="12">
         <v>580</v>
@@ -18586,7 +18580,7 @@
       </c>
       <c r="B581" s="11"/>
       <c r="C581" s="11" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D581" s="12">
         <v>580</v>
@@ -18605,7 +18599,7 @@
       </c>
       <c r="B582" s="11"/>
       <c r="C582" s="11" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D582" s="12">
         <v>580</v>
@@ -18614,7 +18608,7 @@
         <v>580</v>
       </c>
       <c r="F582" s="16" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="G582" s="11"/>
       <c r="H582" s="11"/>
@@ -18626,7 +18620,7 @@
       </c>
       <c r="B583" s="11"/>
       <c r="C583" s="11" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D583" s="12">
         <v>635</v>
@@ -18645,7 +18639,7 @@
       </c>
       <c r="B584" s="11"/>
       <c r="C584" s="11" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="D584" s="12">
         <v>610</v>
@@ -18654,7 +18648,7 @@
         <v>600</v>
       </c>
       <c r="F584" s="20" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="G584" s="11"/>
       <c r="H584" s="11"/>
@@ -18666,7 +18660,7 @@
       </c>
       <c r="B585" s="11"/>
       <c r="C585" s="11" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D585" s="12">
         <v>605</v>
@@ -18675,11 +18669,11 @@
         <v>600</v>
       </c>
       <c r="F585" s="20" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="G585" s="11"/>
       <c r="H585" s="11" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="I585" s="11"/>
     </row>
@@ -18689,7 +18683,7 @@
       </c>
       <c r="B586" s="11"/>
       <c r="C586" s="11" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="D586" s="12">
         <v>690</v>
@@ -18707,7 +18701,7 @@
         <v>583</v>
       </c>
       <c r="C587" s="4" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="D587" s="5">
         <v>610</v>
@@ -18721,7 +18715,7 @@
         <v>584</v>
       </c>
       <c r="C588" s="11" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D588" s="14">
         <v>600</v>
@@ -18735,7 +18729,7 @@
         <v>585</v>
       </c>
       <c r="C589" s="11" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D589" s="14">
         <v>620</v>
@@ -18749,7 +18743,7 @@
         <v>586</v>
       </c>
       <c r="C590" s="11" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D590" s="14">
         <v>620</v>
@@ -18763,7 +18757,7 @@
         <v>587</v>
       </c>
       <c r="C591" s="4" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="D591" s="5">
         <v>680</v>
@@ -18772,7 +18766,7 @@
         <v>670</v>
       </c>
       <c r="F591" s="10" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="592" spans="1:9" x14ac:dyDescent="0.2">
@@ -18780,7 +18774,7 @@
         <v>588</v>
       </c>
       <c r="C592" s="11" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="D592" s="14">
         <v>745</v>
@@ -18794,7 +18788,7 @@
         <v>589</v>
       </c>
       <c r="C593" s="11" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D593" s="14">
         <v>725</v>
@@ -18803,7 +18797,7 @@
         <v>715</v>
       </c>
       <c r="F593" s="2" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="594" spans="1:6" x14ac:dyDescent="0.2">
@@ -18811,7 +18805,7 @@
         <v>590</v>
       </c>
       <c r="C594" s="11" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="D594" s="14">
         <v>740</v>
@@ -18820,7 +18814,7 @@
         <v>730</v>
       </c>
       <c r="F594" s="2" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="595" spans="1:6" x14ac:dyDescent="0.2">
@@ -18828,7 +18822,7 @@
         <v>591</v>
       </c>
       <c r="C595" s="11" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="D595" s="14">
         <v>700</v>
@@ -18837,7 +18831,7 @@
         <v>690</v>
       </c>
       <c r="F595" s="2" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="596" spans="1:6" x14ac:dyDescent="0.2">
@@ -18845,7 +18839,7 @@
         <v>592</v>
       </c>
       <c r="C596" s="11" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D596" s="14">
         <v>750</v>
@@ -18854,7 +18848,7 @@
         <v>735</v>
       </c>
       <c r="F596" s="2" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="597" spans="1:6" x14ac:dyDescent="0.2">
@@ -18862,7 +18856,7 @@
         <v>593</v>
       </c>
       <c r="C597" s="11" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D597" s="14">
         <v>600</v>
@@ -18871,7 +18865,7 @@
         <v>600</v>
       </c>
       <c r="F597" s="2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="598" spans="1:6" x14ac:dyDescent="0.2">
@@ -18879,7 +18873,7 @@
         <v>594</v>
       </c>
       <c r="C598" s="11" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D598" s="14">
         <v>760</v>
@@ -18888,7 +18882,7 @@
         <v>750</v>
       </c>
       <c r="F598" s="2" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="599" spans="1:6" x14ac:dyDescent="0.2">
@@ -18896,7 +18890,7 @@
         <v>595</v>
       </c>
       <c r="C599" s="11" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D599" s="14">
         <v>600</v>
@@ -18905,272 +18899,272 @@
         <v>600</v>
       </c>
       <c r="F599" s="2" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="600" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A600" s="11">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C600" s="11" t="s">
+        <v>1049</v>
+      </c>
+      <c r="D600" s="14">
+        <v>720</v>
+      </c>
+      <c r="E600" s="1">
+        <v>710</v>
+      </c>
+      <c r="F600" s="2" t="s">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A601" s="11">
+        <v>598</v>
+      </c>
+      <c r="C601" s="4" t="s">
         <v>1051</v>
       </c>
-      <c r="D600" s="14">
-        <v>770</v>
-      </c>
-      <c r="E600" s="1">
-        <v>750</v>
-      </c>
-      <c r="F600" s="2" t="s">
-        <v>1052</v>
-      </c>
-    </row>
-    <row r="601" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A601" s="11">
-        <v>597</v>
-      </c>
-      <c r="C601" s="11" t="s">
-        <v>1053</v>
-      </c>
-      <c r="D601" s="14">
-        <v>720</v>
-      </c>
-      <c r="E601" s="1">
-        <v>710</v>
-      </c>
-      <c r="F601" s="2" t="s">
-        <v>1054</v>
+      <c r="D601" s="5">
+        <v>655</v>
+      </c>
+      <c r="E601" s="5">
+        <v>640</v>
+      </c>
+      <c r="F601" s="10" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="602" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A602" s="11">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C602" s="4" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D602" s="5">
-        <v>655</v>
+        <v>750</v>
       </c>
       <c r="E602" s="5">
-        <v>640</v>
-      </c>
-      <c r="F602" s="10" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="603" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="603" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A603" s="11">
-        <v>599</v>
-      </c>
-      <c r="C603" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="C603" s="11" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D603" s="14">
+        <v>760</v>
+      </c>
+      <c r="E603" s="1">
+        <v>740</v>
+      </c>
+      <c r="F603" s="2" t="s">
         <v>1057</v>
-      </c>
-      <c r="D603" s="5">
-        <v>750</v>
-      </c>
-      <c r="E603" s="5">
-        <v>740</v>
       </c>
     </row>
     <row r="604" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A604" s="11">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="C604" s="11" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="D604" s="14">
-        <v>760</v>
+        <v>630</v>
       </c>
       <c r="E604" s="1">
-        <v>740</v>
-      </c>
-      <c r="F604" s="2" t="s">
-        <v>1061</v>
+        <v>620</v>
       </c>
     </row>
     <row r="605" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A605" s="11">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="C605" s="11" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="D605" s="14">
-        <v>630</v>
+        <v>730</v>
       </c>
       <c r="E605" s="1">
-        <v>620</v>
+        <v>715</v>
+      </c>
+      <c r="F605" s="2" t="s">
+        <v>1060</v>
       </c>
     </row>
     <row r="606" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A606" s="11">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C606" s="11" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="D606" s="14">
-        <v>730</v>
+        <v>610</v>
       </c>
       <c r="E606" s="1">
-        <v>715</v>
+        <v>600</v>
       </c>
       <c r="F606" s="2" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="607" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A607" s="11">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C607" s="11" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D607" s="14">
+        <v>730</v>
+      </c>
+      <c r="E607" s="1">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A608" s="11">
+        <v>605</v>
+      </c>
+      <c r="C608" s="4" t="s">
         <v>1065</v>
       </c>
-      <c r="D607" s="14">
-        <v>610</v>
-      </c>
-      <c r="E607" s="1">
-        <v>600</v>
-      </c>
-      <c r="F607" s="2" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="608" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A608" s="11">
-        <v>604</v>
-      </c>
-      <c r="C608" s="11" t="s">
-        <v>1067</v>
-      </c>
-      <c r="D608" s="14">
-        <v>730</v>
-      </c>
-      <c r="E608" s="1">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="609" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D608" s="5">
+        <v>685</v>
+      </c>
+      <c r="E608" s="5">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A609" s="11">
-        <v>605</v>
-      </c>
-      <c r="C609" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D609" s="5">
-        <v>685</v>
-      </c>
-      <c r="E609" s="5">
-        <v>670</v>
+        <v>606</v>
+      </c>
+      <c r="C609" s="11" t="s">
+        <v>1078</v>
+      </c>
+      <c r="D609" s="14">
+        <v>625</v>
+      </c>
+      <c r="E609" s="1">
+        <v>615</v>
+      </c>
+      <c r="F609" s="2" t="s">
+        <v>1079</v>
       </c>
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A610" s="11">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C610" s="11" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
       <c r="D610" s="14">
-        <v>625</v>
+        <v>645</v>
       </c>
       <c r="E610" s="1">
-        <v>615</v>
+        <v>635</v>
       </c>
       <c r="F610" s="2" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="611" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A611" s="11">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C611" s="11" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
       <c r="D611" s="14">
-        <v>645</v>
+        <v>600</v>
       </c>
       <c r="E611" s="1">
-        <v>635</v>
-      </c>
-      <c r="F611" s="2" t="s">
-        <v>1085</v>
+        <v>600</v>
       </c>
     </row>
     <row r="612" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A612" s="11">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="C612" s="11" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="D612" s="14">
-        <v>600</v>
+        <v>660</v>
       </c>
       <c r="E612" s="1">
-        <v>600</v>
+        <v>655</v>
+      </c>
+      <c r="F612" s="2" t="s">
+        <v>1084</v>
       </c>
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A613" s="11">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="C613" s="11" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="D613" s="14">
-        <v>660</v>
+        <v>590</v>
       </c>
       <c r="E613" s="1">
-        <v>655</v>
+        <v>590</v>
       </c>
       <c r="F613" s="2" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="614" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A614" s="11">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C614" s="11" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="D614" s="14">
-        <v>590</v>
+        <v>620</v>
       </c>
       <c r="E614" s="1">
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="F614" s="2" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="615" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A615" s="11">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="C615" s="11" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="D615" s="14">
-        <v>620</v>
+        <v>640</v>
       </c>
       <c r="E615" s="1">
-        <v>600</v>
+        <v>630</v>
       </c>
       <c r="F615" s="2" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="616" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A616" s="11">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C616" s="11" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D616" s="14">
         <v>640</v>
@@ -19179,63 +19173,60 @@
         <v>630</v>
       </c>
       <c r="F616" s="2" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="617" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A617" s="11">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C617" s="11" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
       <c r="D617" s="14">
         <v>640</v>
       </c>
       <c r="E617" s="1">
-        <v>630</v>
-      </c>
-      <c r="F617" s="2" t="s">
-        <v>1096</v>
+        <v>625</v>
       </c>
     </row>
     <row r="618" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A618" s="11">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="C618" s="11" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
       <c r="D618" s="14">
-        <v>640</v>
+        <v>615</v>
       </c>
       <c r="E618" s="1">
-        <v>625</v>
+        <v>605</v>
+      </c>
+      <c r="F618" s="2" t="s">
+        <v>1095</v>
       </c>
     </row>
     <row r="619" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A619" s="11">
+        <v>616</v>
+      </c>
+      <c r="C619" s="11" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D619" s="14">
+        <v>625</v>
+      </c>
+      <c r="E619" s="1">
         <v>615</v>
-      </c>
-      <c r="C619" s="11" t="s">
-        <v>1098</v>
-      </c>
-      <c r="D619" s="14">
-        <v>615</v>
-      </c>
-      <c r="E619" s="1">
-        <v>605</v>
-      </c>
-      <c r="F619" s="2" t="s">
-        <v>1099</v>
       </c>
     </row>
     <row r="620" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A620" s="11">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C620" s="11" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="D620" s="14">
         <v>625</v>
@@ -19246,106 +19237,106 @@
     </row>
     <row r="621" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A621" s="11">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="C621" s="11" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
       <c r="D621" s="14">
-        <v>625</v>
+        <v>600</v>
       </c>
       <c r="E621" s="1">
-        <v>615</v>
+        <v>600</v>
+      </c>
+      <c r="F621" s="2" t="s">
+        <v>1099</v>
       </c>
     </row>
     <row r="622" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A622" s="11">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C622" s="11" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="D622" s="14">
-        <v>600</v>
+        <v>625</v>
       </c>
       <c r="E622" s="1">
-        <v>600</v>
-      </c>
-      <c r="F622" s="2" t="s">
-        <v>1103</v>
+        <v>615</v>
       </c>
     </row>
     <row r="623" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A623" s="11">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="C623" s="11" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="D623" s="14">
-        <v>625</v>
+        <v>600</v>
       </c>
       <c r="E623" s="1">
-        <v>615</v>
+        <v>600</v>
       </c>
     </row>
     <row r="624" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A624" s="11">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C624" s="11" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="D624" s="14">
-        <v>600</v>
+        <v>610</v>
       </c>
       <c r="E624" s="1">
         <v>600</v>
       </c>
+      <c r="F624" s="2" t="s">
+        <v>1103</v>
+      </c>
     </row>
     <row r="625" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A625" s="11">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C625" s="11" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="D625" s="14">
-        <v>610</v>
+        <v>635</v>
       </c>
       <c r="E625" s="1">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="F625" s="2" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="626" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A626" s="11">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="C626" s="11" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="D626" s="14">
-        <v>635</v>
+        <v>600</v>
       </c>
       <c r="E626" s="1">
-        <v>620</v>
-      </c>
-      <c r="F626" s="2" t="s">
-        <v>1109</v>
+        <v>600</v>
       </c>
     </row>
     <row r="627" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A627" s="11">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="C627" s="11" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="D627" s="14">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E627" s="1">
         <v>600</v>
@@ -19353,89 +19344,89 @@
     </row>
     <row r="628" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A628" s="11">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C628" s="11" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="D628" s="14">
-        <v>605</v>
+        <v>635</v>
       </c>
       <c r="E628" s="1">
-        <v>600</v>
+        <v>625</v>
       </c>
     </row>
     <row r="629" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A629" s="11">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="C629" s="11" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="D629" s="14">
-        <v>635</v>
+        <v>605</v>
       </c>
       <c r="E629" s="1">
-        <v>625</v>
+        <v>600</v>
+      </c>
+      <c r="F629" s="2" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="630" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A630" s="11">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="C630" s="11" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D630" s="14">
-        <v>605</v>
+        <v>650</v>
       </c>
       <c r="E630" s="1">
-        <v>600</v>
+        <v>640</v>
       </c>
       <c r="F630" s="2" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="631" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A631" s="11">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="C631" s="11" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D631" s="14">
-        <v>650</v>
+        <v>640</v>
       </c>
       <c r="E631" s="1">
-        <v>640</v>
-      </c>
-      <c r="F631" s="2" t="s">
-        <v>1116</v>
+        <v>630</v>
       </c>
     </row>
     <row r="632" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A632" s="11">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="C632" s="11" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="D632" s="14">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="E632" s="1">
-        <v>630</v>
+        <v>600</v>
       </c>
     </row>
     <row r="633" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A633" s="11">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C633" s="11" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="D633" s="14">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E633" s="1">
         <v>600</v>
@@ -19443,75 +19434,78 @@
     </row>
     <row r="634" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A634" s="11">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="C634" s="11" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="D634" s="14">
-        <v>605</v>
+        <v>640</v>
       </c>
       <c r="E634" s="1">
-        <v>600</v>
+        <v>635</v>
+      </c>
+      <c r="F634" s="2" t="s">
+        <v>1117</v>
       </c>
     </row>
     <row r="635" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A635" s="11">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="C635" s="11" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
       <c r="D635" s="14">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="E635" s="1">
-        <v>635</v>
-      </c>
-      <c r="F635" s="2" t="s">
-        <v>1121</v>
+        <v>630</v>
       </c>
     </row>
     <row r="636" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A636" s="11">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="C636" s="11" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
       <c r="D636" s="14">
-        <v>635</v>
+        <v>600</v>
       </c>
       <c r="E636" s="1">
-        <v>630</v>
+        <v>600</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A637" s="11">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="C637" s="11" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="D637" s="14">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="E637" s="1">
         <v>600</v>
       </c>
+      <c r="F637" s="2" t="s">
+        <v>1130</v>
+      </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A638" s="11">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="C638" s="11" t="s">
         <v>1133</v>
       </c>
       <c r="D638" s="14">
-        <v>605</v>
+        <v>630</v>
       </c>
       <c r="E638" s="1">
-        <v>600</v>
+        <v>620</v>
       </c>
       <c r="F638" s="2" t="s">
         <v>1134</v>
@@ -19519,63 +19513,46 @@
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A639" s="11">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C639" s="11" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D639" s="14">
-        <v>630</v>
+        <v>620</v>
       </c>
       <c r="E639" s="1">
-        <v>620</v>
+        <v>610</v>
       </c>
       <c r="F639" s="2" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="640" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A640" s="11">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="C640" s="11" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="D640" s="14">
+        <v>625</v>
+      </c>
+      <c r="E640" s="1">
         <v>620</v>
-      </c>
-      <c r="E640" s="1">
-        <v>610</v>
-      </c>
-      <c r="F640" s="2" t="s">
-        <v>1140</v>
       </c>
     </row>
     <row r="641" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A641" s="11">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="C641" s="11" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D641" s="14">
-        <v>625</v>
+        <v>680</v>
       </c>
       <c r="E641" s="1">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="642" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A642" s="11">
-        <v>638</v>
-      </c>
-      <c r="C642" s="11" t="s">
-        <v>1143</v>
-      </c>
-      <c r="D642" s="14">
-        <v>680</v>
-      </c>
-      <c r="E642" s="1">
         <v>660</v>
       </c>
     </row>
@@ -19693,7 +19670,7 @@
         <v>560</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -19731,7 +19708,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="D9" s="22">
         <v>635</v>
@@ -19851,7 +19828,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D17" s="7">
         <v>690</v>
@@ -19868,7 +19845,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="D18" s="5">
         <v>675</v>
@@ -20232,7 +20209,7 @@
         <v>36</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="D41" s="5">
         <v>660</v>
@@ -20559,7 +20536,7 @@
         <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="D63" s="1">
         <v>600</v>
@@ -20568,7 +20545,7 @@
         <v>590</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -20576,7 +20553,7 @@
         <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D64" s="1">
         <v>590</v>
@@ -20585,7 +20562,7 @@
         <v>580</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -20593,7 +20570,7 @@
         <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="D65" s="1">
         <v>725</v>
@@ -20607,7 +20584,7 @@
         <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D66" s="1">
         <v>720</v>
@@ -20616,7 +20593,7 @@
         <v>700</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
@@ -20624,7 +20601,7 @@
         <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D67" s="1">
         <v>600</v>
@@ -20633,7 +20610,7 @@
         <v>585</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="68" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -20641,7 +20618,7 @@
         <v>63</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="D68" s="7">
         <v>645</v>
@@ -20650,7 +20627,7 @@
         <v>640</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -20658,7 +20635,7 @@
         <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="D69" s="1">
         <v>585</v>
@@ -20667,7 +20644,7 @@
         <v>575</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -20675,7 +20652,7 @@
         <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D70" s="1">
         <v>615</v>
@@ -20684,7 +20661,7 @@
         <v>610</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -20692,7 +20669,7 @@
         <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="D71" s="1">
         <v>620</v>
@@ -20701,7 +20678,7 @@
         <v>610</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -20709,7 +20686,7 @@
         <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="D72" s="1">
         <v>610</v>
@@ -20724,7 +20701,7 @@
         <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="D73" s="1">
         <v>650</v>
@@ -20739,7 +20716,7 @@
         <v>69</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D74" s="5">
         <v>615</v>
@@ -20754,7 +20731,7 @@
         <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="D75" s="1">
         <v>640</v>
@@ -20769,7 +20746,7 @@
         <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="D76" s="1">
         <v>615</v>
@@ -20778,7 +20755,7 @@
         <v>600</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -20786,7 +20763,7 @@
         <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="D77" s="1">
         <v>600</v>
@@ -20795,7 +20772,7 @@
         <v>590</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="78" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -20803,7 +20780,7 @@
         <v>73</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="D78" s="12">
         <v>635</v>
@@ -20817,7 +20794,7 @@
         <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D79" s="1">
         <v>700</v>
@@ -20832,7 +20809,7 @@
         <v>75</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="D80" s="7">
         <v>680</v>
@@ -20847,7 +20824,7 @@
         <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D81" s="1">
         <v>620</v>
@@ -20856,7 +20833,7 @@
         <v>610</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -20864,7 +20841,7 @@
         <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="D82" s="1">
         <v>645</v>
@@ -20873,7 +20850,7 @@
         <v>635</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -20881,7 +20858,7 @@
         <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="D83" s="1">
         <v>600</v>
@@ -20895,7 +20872,7 @@
         <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="D84" s="1">
         <v>615</v>
@@ -20909,7 +20886,7 @@
         <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
       <c r="D85" s="1">
         <v>580</v>
@@ -20918,7 +20895,7 @@
         <v>570</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -20926,7 +20903,7 @@
         <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="D86" s="1">
         <v>640</v>
@@ -20941,7 +20918,7 @@
         <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="D87" s="1">
         <v>575</v>
@@ -20950,7 +20927,7 @@
         <v>570</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -20958,7 +20935,7 @@
         <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="D88" s="1">
         <v>580</v>
@@ -20973,7 +20950,7 @@
         <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="D89" s="1">
         <v>690</v>
@@ -20982,7 +20959,7 @@
         <v>670</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1080</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -20990,7 +20967,7 @@
         <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="D90" s="1">
         <v>575</v>
@@ -20999,7 +20976,7 @@
         <v>570</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>1125</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix: add Nam San Bay
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/per-github/project-tennis/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBE95B3-40D9-FD42-80F7-181C73D8DBE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF8CAB-E48D-1B40-8262-64D72DD15352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="25320" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1266" uniqueCount="1142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="1143">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -4289,28 +4289,6 @@
   </si>
   <si>
     <r>
-      <t>Tu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>ấ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">n 276 </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>C</t>
     </r>
     <r>
@@ -6404,6 +6382,12 @@
   </si>
   <si>
     <t>La Costa</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn</t>
+  </si>
+  <si>
+    <t>Nam Sân Bay</t>
   </si>
 </sst>
 </file>
@@ -6830,10 +6814,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I640"/>
+  <dimension ref="A1:I641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="C250" sqref="C250"/>
+    <sheetView tabSelected="1" topLeftCell="A619" workbookViewId="0">
+      <selection activeCell="E639" sqref="E639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7014,10 +6998,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="D10" s="7">
         <v>600</v>
@@ -7110,7 +7094,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="D14" s="7">
         <v>650</v>
@@ -7381,7 +7365,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>1135</v>
+        <v>1134</v>
       </c>
       <c r="D26" s="22">
         <v>640</v>
@@ -7470,7 +7454,7 @@
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D30" s="12">
         <v>605</v>
@@ -7602,7 +7586,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D36" s="5">
         <v>605</v>
@@ -7643,7 +7627,7 @@
         <v>33</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="D38" s="7">
         <v>615</v>
@@ -8046,7 +8030,7 @@
         <v>53</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="D58" s="5">
         <v>650</v>
@@ -9068,7 +9052,7 @@
         <v>102</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="D107" s="7">
         <v>605</v>
@@ -9309,7 +9293,7 @@
       </c>
       <c r="B119" s="11"/>
       <c r="C119" s="11" t="s">
-        <v>975</v>
+        <v>1141</v>
       </c>
       <c r="D119" s="12">
         <v>600</v>
@@ -9332,7 +9316,7 @@
       </c>
       <c r="B120" s="11"/>
       <c r="C120" s="11" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="D120" s="12">
         <v>600</v>
@@ -9376,7 +9360,7 @@
       </c>
       <c r="B122" s="11"/>
       <c r="C122" s="11" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="D122" s="12">
         <v>645</v>
@@ -9399,7 +9383,7 @@
       </c>
       <c r="B123" s="11"/>
       <c r="C123" s="11" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="D123" s="12">
         <v>590</v>
@@ -9418,7 +9402,7 @@
       </c>
       <c r="B124" s="11"/>
       <c r="C124" s="11" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D124" s="12">
         <v>615</v>
@@ -9437,7 +9421,7 @@
       </c>
       <c r="B125" s="11"/>
       <c r="C125" s="11" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D125" s="12">
         <v>635</v>
@@ -9499,7 +9483,7 @@
         <v>123</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="D128" s="5">
         <v>635</v>
@@ -9517,7 +9501,7 @@
       </c>
       <c r="B129" s="11"/>
       <c r="C129" s="11" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="D129" s="12">
         <v>610</v>
@@ -9555,7 +9539,7 @@
       </c>
       <c r="B131" s="11"/>
       <c r="C131" s="11" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D131" s="12">
         <v>680</v>
@@ -9574,7 +9558,7 @@
       </c>
       <c r="B132" s="11"/>
       <c r="C132" s="11" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="D132" s="12">
         <v>590</v>
@@ -9616,7 +9600,7 @@
       </c>
       <c r="B134" s="11"/>
       <c r="C134" s="11" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D134" s="12">
         <v>635</v>
@@ -9637,7 +9621,7 @@
       </c>
       <c r="B135" s="11"/>
       <c r="C135" s="11" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
       <c r="D135" s="12">
         <v>610</v>
@@ -9754,7 +9738,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D141" s="7">
         <v>765</v>
@@ -9772,7 +9756,7 @@
       </c>
       <c r="B142" s="11"/>
       <c r="C142" s="11" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D142" s="12">
         <v>785</v>
@@ -9810,7 +9794,7 @@
       </c>
       <c r="B144" s="11"/>
       <c r="C144" s="11" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D144" s="12">
         <v>985</v>
@@ -9850,7 +9834,7 @@
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="11" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D146" s="12">
         <v>850</v>
@@ -9888,7 +9872,7 @@
       </c>
       <c r="B148" s="11"/>
       <c r="C148" s="11" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D148" s="12">
         <v>790</v>
@@ -9906,7 +9890,7 @@
         <v>144</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="D149" s="7">
         <v>760</v>
@@ -9961,7 +9945,7 @@
       </c>
       <c r="B152" s="11"/>
       <c r="C152" s="11" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D152" s="12">
         <v>840</v>
@@ -9982,7 +9966,7 @@
       </c>
       <c r="B153" s="11"/>
       <c r="C153" s="11" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="D153" s="12">
         <v>785</v>
@@ -10001,7 +9985,7 @@
       </c>
       <c r="B154" s="11"/>
       <c r="C154" s="11" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="D154" s="12">
         <v>880</v>
@@ -10041,7 +10025,7 @@
       </c>
       <c r="B156" s="11"/>
       <c r="C156" s="11" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="D156" s="12">
         <v>830</v>
@@ -10062,7 +10046,7 @@
       </c>
       <c r="B157" s="11"/>
       <c r="C157" s="11" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D157" s="12">
         <v>935</v>
@@ -10121,7 +10105,7 @@
       </c>
       <c r="B160" s="11"/>
       <c r="C160" s="11" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D160" s="12">
         <v>920</v>
@@ -10180,7 +10164,7 @@
       </c>
       <c r="B163" s="11"/>
       <c r="C163" s="11" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D163" s="12">
         <v>810</v>
@@ -10201,7 +10185,7 @@
       </c>
       <c r="B164" s="11"/>
       <c r="C164" s="11" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D164" s="12">
         <v>755</v>
@@ -10222,7 +10206,7 @@
       </c>
       <c r="B165" s="11"/>
       <c r="C165" s="11" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D165" s="12">
         <v>605</v>
@@ -10241,7 +10225,7 @@
       </c>
       <c r="B166" s="11"/>
       <c r="C166" s="11" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D166" s="12">
         <v>990</v>
@@ -10280,7 +10264,7 @@
         <v>163</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="D168" s="7">
         <v>735</v>
@@ -10298,7 +10282,7 @@
       </c>
       <c r="B169" s="11"/>
       <c r="C169" s="11" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D169" s="12">
         <v>630</v>
@@ -10340,7 +10324,7 @@
       </c>
       <c r="B171" s="11"/>
       <c r="C171" s="11" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D171" s="12">
         <v>750</v>
@@ -10422,7 +10406,7 @@
       </c>
       <c r="B175" s="11"/>
       <c r="C175" s="11" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D175" s="12">
         <v>910</v>
@@ -10462,7 +10446,7 @@
       </c>
       <c r="B177" s="11"/>
       <c r="C177" s="11" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D177" s="12">
         <v>930</v>
@@ -10483,7 +10467,7 @@
       </c>
       <c r="B178" s="11"/>
       <c r="C178" s="11" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="D178" s="12">
         <v>955</v>
@@ -10504,7 +10488,7 @@
       </c>
       <c r="B179" s="11"/>
       <c r="C179" s="11" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="D179" s="12">
         <v>1010</v>
@@ -10525,7 +10509,7 @@
       </c>
       <c r="B180" s="11"/>
       <c r="C180" s="11" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="D180" s="12">
         <v>670</v>
@@ -10565,7 +10549,7 @@
       </c>
       <c r="B182" s="11"/>
       <c r="C182" s="11" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="D182" s="12">
         <v>890</v>
@@ -10584,7 +10568,7 @@
       </c>
       <c r="B183" s="11"/>
       <c r="C183" s="11" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D183" s="12">
         <v>815</v>
@@ -10603,7 +10587,7 @@
       </c>
       <c r="B184" s="11"/>
       <c r="C184" s="11" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D184" s="12">
         <v>835</v>
@@ -10624,7 +10608,7 @@
       </c>
       <c r="B185" s="11"/>
       <c r="C185" s="11" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D185" s="12">
         <v>735</v>
@@ -10645,7 +10629,7 @@
       </c>
       <c r="B186" s="11"/>
       <c r="C186" s="11" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D186" s="12">
         <v>780</v>
@@ -10664,7 +10648,7 @@
       </c>
       <c r="B187" s="11"/>
       <c r="C187" s="11" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="D187" s="12">
         <v>810</v>
@@ -10683,7 +10667,7 @@
       </c>
       <c r="B188" s="11"/>
       <c r="C188" s="11" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="D188" s="12">
         <v>880</v>
@@ -10704,7 +10688,7 @@
       </c>
       <c r="B189" s="11"/>
       <c r="C189" s="11" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="D189" s="12">
         <v>885</v>
@@ -10724,7 +10708,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D190" s="7">
         <v>695</v>
@@ -10758,7 +10742,7 @@
       </c>
       <c r="B192" s="11"/>
       <c r="C192" s="11" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="D192" s="12">
         <v>880</v>
@@ -10779,7 +10763,7 @@
       </c>
       <c r="B193" s="11"/>
       <c r="C193" s="11" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D193" s="12">
         <v>745</v>
@@ -10838,7 +10822,7 @@
       </c>
       <c r="B196" s="11"/>
       <c r="C196" s="11" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D196" s="12">
         <v>790</v>
@@ -10874,7 +10858,7 @@
       </c>
       <c r="B198" s="11"/>
       <c r="C198" s="11" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
       <c r="D198" s="12">
         <v>740</v>
@@ -10893,7 +10877,7 @@
       </c>
       <c r="B199" s="11"/>
       <c r="C199" s="11" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D199" s="12">
         <v>730</v>
@@ -10912,7 +10896,7 @@
       </c>
       <c r="B200" s="11"/>
       <c r="C200" s="11" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D200" s="12">
         <v>745</v>
@@ -10945,7 +10929,7 @@
       </c>
       <c r="B202" s="11"/>
       <c r="C202" s="11" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D202" s="12">
         <v>660</v>
@@ -11022,7 +11006,7 @@
         <v>201</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="D206" s="7">
         <v>690</v>
@@ -11056,7 +11040,7 @@
       </c>
       <c r="B208" s="11"/>
       <c r="C208" s="11" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D208" s="12">
         <v>760</v>
@@ -11075,7 +11059,7 @@
       </c>
       <c r="B209" s="11"/>
       <c r="C209" s="11" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D209" s="12">
         <v>725</v>
@@ -12107,7 +12091,7 @@
       </c>
       <c r="B256" s="11"/>
       <c r="C256" s="11" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
       <c r="D256" s="12">
         <v>645</v>
@@ -16247,7 +16231,7 @@
       </c>
       <c r="B462" s="11"/>
       <c r="C462" s="11" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="D462" s="12">
         <v>615</v>
@@ -16256,7 +16240,7 @@
         <v>615</v>
       </c>
       <c r="F462" s="16" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="G462" s="11"/>
       <c r="H462" s="11"/>
@@ -17662,7 +17646,7 @@
       </c>
       <c r="B534" s="11"/>
       <c r="C534" s="11" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D534" s="12">
         <v>760</v>
@@ -18682,7 +18666,7 @@
         <v>583</v>
       </c>
       <c r="C586" s="4" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D586" s="5">
         <v>610</v>
@@ -18696,7 +18680,7 @@
         <v>584</v>
       </c>
       <c r="C587" s="11" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="D587" s="14">
         <v>600</v>
@@ -18710,7 +18694,7 @@
         <v>585</v>
       </c>
       <c r="C588" s="11" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D588" s="14">
         <v>620</v>
@@ -18724,7 +18708,7 @@
         <v>586</v>
       </c>
       <c r="C589" s="11" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D589" s="14">
         <v>620</v>
@@ -18738,7 +18722,7 @@
         <v>587</v>
       </c>
       <c r="C590" s="4" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D590" s="5">
         <v>680</v>
@@ -18747,7 +18731,7 @@
         <v>670</v>
       </c>
       <c r="F590" s="10" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.2">
@@ -18755,7 +18739,7 @@
         <v>588</v>
       </c>
       <c r="C591" s="11" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D591" s="14">
         <v>745</v>
@@ -18769,7 +18753,7 @@
         <v>589</v>
       </c>
       <c r="C592" s="11" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D592" s="14">
         <v>725</v>
@@ -18778,7 +18762,7 @@
         <v>715</v>
       </c>
       <c r="F592" s="2" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="593" spans="1:6" x14ac:dyDescent="0.2">
@@ -18786,7 +18770,7 @@
         <v>590</v>
       </c>
       <c r="C593" s="11" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D593" s="14">
         <v>740</v>
@@ -18795,7 +18779,7 @@
         <v>730</v>
       </c>
       <c r="F593" s="2" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="594" spans="1:6" x14ac:dyDescent="0.2">
@@ -18803,7 +18787,7 @@
         <v>591</v>
       </c>
       <c r="C594" s="11" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D594" s="14">
         <v>700</v>
@@ -18812,7 +18796,7 @@
         <v>690</v>
       </c>
       <c r="F594" s="2" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="595" spans="1:6" x14ac:dyDescent="0.2">
@@ -18820,7 +18804,7 @@
         <v>592</v>
       </c>
       <c r="C595" s="11" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D595" s="14">
         <v>750</v>
@@ -18829,7 +18813,7 @@
         <v>735</v>
       </c>
       <c r="F595" s="2" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="596" spans="1:6" x14ac:dyDescent="0.2">
@@ -18837,7 +18821,7 @@
         <v>593</v>
       </c>
       <c r="C596" s="11" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D596" s="14">
         <v>600</v>
@@ -18846,7 +18830,7 @@
         <v>600</v>
       </c>
       <c r="F596" s="2" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="597" spans="1:6" x14ac:dyDescent="0.2">
@@ -18854,7 +18838,7 @@
         <v>594</v>
       </c>
       <c r="C597" s="11" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D597" s="14">
         <v>760</v>
@@ -18863,7 +18847,7 @@
         <v>750</v>
       </c>
       <c r="F597" s="2" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="598" spans="1:6" x14ac:dyDescent="0.2">
@@ -18871,7 +18855,7 @@
         <v>595</v>
       </c>
       <c r="C598" s="11" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D598" s="14">
         <v>600</v>
@@ -18880,7 +18864,7 @@
         <v>600</v>
       </c>
       <c r="F598" s="2" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="599" spans="1:6" x14ac:dyDescent="0.2">
@@ -18888,7 +18872,7 @@
         <v>597</v>
       </c>
       <c r="C599" s="11" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D599" s="14">
         <v>720</v>
@@ -18897,7 +18881,7 @@
         <v>710</v>
       </c>
       <c r="F599" s="2" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="600" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -18905,7 +18889,7 @@
         <v>598</v>
       </c>
       <c r="C600" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="D600" s="5">
         <v>655</v>
@@ -18922,7 +18906,7 @@
         <v>599</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D601" s="5">
         <v>750</v>
@@ -18936,7 +18920,7 @@
         <v>600</v>
       </c>
       <c r="C602" s="11" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="D602" s="14">
         <v>760</v>
@@ -18945,7 +18929,7 @@
         <v>740</v>
       </c>
       <c r="F602" s="2" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="603" spans="1:6" x14ac:dyDescent="0.2">
@@ -18953,7 +18937,7 @@
         <v>601</v>
       </c>
       <c r="C603" s="11" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D603" s="14">
         <v>630</v>
@@ -18967,7 +18951,7 @@
         <v>602</v>
       </c>
       <c r="C604" s="11" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D604" s="14">
         <v>730</v>
@@ -18976,7 +18960,7 @@
         <v>715</v>
       </c>
       <c r="F604" s="2" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="605" spans="1:6" x14ac:dyDescent="0.2">
@@ -18984,7 +18968,7 @@
         <v>603</v>
       </c>
       <c r="C605" s="11" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="D605" s="14">
         <v>610</v>
@@ -18993,7 +18977,7 @@
         <v>600</v>
       </c>
       <c r="F605" s="2" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="606" spans="1:6" x14ac:dyDescent="0.2">
@@ -19001,7 +18985,7 @@
         <v>604</v>
       </c>
       <c r="C606" s="11" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="D606" s="14">
         <v>730</v>
@@ -19015,7 +18999,7 @@
         <v>605</v>
       </c>
       <c r="C607" s="4" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D607" s="5">
         <v>685</v>
@@ -19029,7 +19013,7 @@
         <v>606</v>
       </c>
       <c r="C608" s="11" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="D608" s="14">
         <v>625</v>
@@ -19038,7 +19022,7 @@
         <v>615</v>
       </c>
       <c r="F608" s="2" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="609" spans="1:6" x14ac:dyDescent="0.2">
@@ -19046,7 +19030,7 @@
         <v>607</v>
       </c>
       <c r="C609" s="11" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="D609" s="14">
         <v>645</v>
@@ -19055,7 +19039,7 @@
         <v>635</v>
       </c>
       <c r="F609" s="2" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.2">
@@ -19063,7 +19047,7 @@
         <v>608</v>
       </c>
       <c r="C610" s="11" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D610" s="14">
         <v>600</v>
@@ -19077,7 +19061,7 @@
         <v>609</v>
       </c>
       <c r="C611" s="11" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="D611" s="14">
         <v>660</v>
@@ -19086,7 +19070,7 @@
         <v>655</v>
       </c>
       <c r="F611" s="2" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="612" spans="1:6" x14ac:dyDescent="0.2">
@@ -19094,7 +19078,7 @@
         <v>610</v>
       </c>
       <c r="C612" s="11" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="D612" s="14">
         <v>590</v>
@@ -19103,7 +19087,7 @@
         <v>590</v>
       </c>
       <c r="F612" s="2" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.2">
@@ -19111,7 +19095,7 @@
         <v>611</v>
       </c>
       <c r="C613" s="11" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="D613" s="14">
         <v>620</v>
@@ -19120,7 +19104,7 @@
         <v>600</v>
       </c>
       <c r="F613" s="2" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="614" spans="1:6" x14ac:dyDescent="0.2">
@@ -19128,7 +19112,7 @@
         <v>612</v>
       </c>
       <c r="C614" s="11" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D614" s="14">
         <v>640</v>
@@ -19137,7 +19121,7 @@
         <v>630</v>
       </c>
       <c r="F614" s="2" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="615" spans="1:6" x14ac:dyDescent="0.2">
@@ -19145,7 +19129,7 @@
         <v>613</v>
       </c>
       <c r="C615" s="11" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="D615" s="14">
         <v>640</v>
@@ -19154,7 +19138,7 @@
         <v>630</v>
       </c>
       <c r="F615" s="2" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="616" spans="1:6" x14ac:dyDescent="0.2">
@@ -19162,7 +19146,7 @@
         <v>614</v>
       </c>
       <c r="C616" s="11" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="D616" s="14">
         <v>640</v>
@@ -19176,7 +19160,7 @@
         <v>615</v>
       </c>
       <c r="C617" s="11" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="D617" s="14">
         <v>615</v>
@@ -19185,7 +19169,7 @@
         <v>605</v>
       </c>
       <c r="F617" s="2" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="618" spans="1:6" x14ac:dyDescent="0.2">
@@ -19193,7 +19177,7 @@
         <v>616</v>
       </c>
       <c r="C618" s="11" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="D618" s="14">
         <v>625</v>
@@ -19207,7 +19191,7 @@
         <v>617</v>
       </c>
       <c r="C619" s="11" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="D619" s="14">
         <v>625</v>
@@ -19221,7 +19205,7 @@
         <v>618</v>
       </c>
       <c r="C620" s="11" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="D620" s="14">
         <v>600</v>
@@ -19230,7 +19214,7 @@
         <v>600</v>
       </c>
       <c r="F620" s="2" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="621" spans="1:6" x14ac:dyDescent="0.2">
@@ -19238,7 +19222,7 @@
         <v>619</v>
       </c>
       <c r="C621" s="11" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D621" s="14">
         <v>625</v>
@@ -19252,7 +19236,7 @@
         <v>620</v>
       </c>
       <c r="C622" s="11" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="D622" s="14">
         <v>600</v>
@@ -19266,7 +19250,7 @@
         <v>621</v>
       </c>
       <c r="C623" s="11" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="D623" s="14">
         <v>610</v>
@@ -19275,7 +19259,7 @@
         <v>600</v>
       </c>
       <c r="F623" s="2" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="624" spans="1:6" x14ac:dyDescent="0.2">
@@ -19283,7 +19267,7 @@
         <v>622</v>
       </c>
       <c r="C624" s="11" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="D624" s="14">
         <v>635</v>
@@ -19292,7 +19276,7 @@
         <v>620</v>
       </c>
       <c r="F624" s="2" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="625" spans="1:6" x14ac:dyDescent="0.2">
@@ -19300,7 +19284,7 @@
         <v>623</v>
       </c>
       <c r="C625" s="11" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="D625" s="14">
         <v>600</v>
@@ -19314,7 +19298,7 @@
         <v>624</v>
       </c>
       <c r="C626" s="11" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="D626" s="14">
         <v>605</v>
@@ -19328,7 +19312,7 @@
         <v>625</v>
       </c>
       <c r="C627" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="D627" s="14">
         <v>635</v>
@@ -19342,7 +19326,7 @@
         <v>626</v>
       </c>
       <c r="C628" s="11" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D628" s="14">
         <v>605</v>
@@ -19351,7 +19335,7 @@
         <v>600</v>
       </c>
       <c r="F628" s="2" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="629" spans="1:6" x14ac:dyDescent="0.2">
@@ -19359,7 +19343,7 @@
         <v>627</v>
       </c>
       <c r="C629" s="11" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D629" s="14">
         <v>650</v>
@@ -19368,7 +19352,7 @@
         <v>640</v>
       </c>
       <c r="F629" s="2" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="630" spans="1:6" x14ac:dyDescent="0.2">
@@ -19376,7 +19360,7 @@
         <v>628</v>
       </c>
       <c r="C630" s="11" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="D630" s="14">
         <v>640</v>
@@ -19390,7 +19374,7 @@
         <v>629</v>
       </c>
       <c r="C631" s="11" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="D631" s="14">
         <v>600</v>
@@ -19404,7 +19388,7 @@
         <v>630</v>
       </c>
       <c r="C632" s="11" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="D632" s="14">
         <v>605</v>
@@ -19418,7 +19402,7 @@
         <v>631</v>
       </c>
       <c r="C633" s="11" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="D633" s="14">
         <v>640</v>
@@ -19427,7 +19411,7 @@
         <v>635</v>
       </c>
       <c r="F633" s="2" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="634" spans="1:6" x14ac:dyDescent="0.2">
@@ -19435,7 +19419,7 @@
         <v>632</v>
       </c>
       <c r="C634" s="11" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="D634" s="14">
         <v>635</v>
@@ -19449,7 +19433,7 @@
         <v>633</v>
       </c>
       <c r="C635" s="11" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="D635" s="14">
         <v>600</v>
@@ -19463,7 +19447,7 @@
         <v>634</v>
       </c>
       <c r="C636" s="11" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="D636" s="14">
         <v>605</v>
@@ -19472,7 +19456,7 @@
         <v>600</v>
       </c>
       <c r="F636" s="2" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.2">
@@ -19480,7 +19464,7 @@
         <v>635</v>
       </c>
       <c r="C637" s="11" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="D637" s="14">
         <v>630</v>
@@ -19489,7 +19473,7 @@
         <v>620</v>
       </c>
       <c r="F637" s="2" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.2">
@@ -19497,7 +19481,7 @@
         <v>636</v>
       </c>
       <c r="C638" s="11" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="D638" s="14">
         <v>620</v>
@@ -19506,7 +19490,7 @@
         <v>610</v>
       </c>
       <c r="F638" s="2" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.2">
@@ -19514,7 +19498,7 @@
         <v>637</v>
       </c>
       <c r="C639" s="11" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="D639" s="14">
         <v>625</v>
@@ -19528,13 +19512,27 @@
         <v>638</v>
       </c>
       <c r="C640" s="11" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D640" s="14">
         <v>680</v>
       </c>
       <c r="E640" s="1">
         <v>660</v>
+      </c>
+    </row>
+    <row r="641" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A641" s="11">
+        <v>639</v>
+      </c>
+      <c r="C641" s="11" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D641" s="14">
+        <v>625</v>
+      </c>
+      <c r="E641" s="1">
+        <v>625</v>
       </c>
     </row>
   </sheetData>
@@ -19689,7 +19687,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="D9" s="22">
         <v>635</v>
@@ -19809,7 +19807,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="D17" s="7">
         <v>690</v>
@@ -19826,7 +19824,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D18" s="5">
         <v>675</v>
@@ -20822,7 +20820,7 @@
         <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D82" s="1">
         <v>645</v>
@@ -20831,7 +20829,7 @@
         <v>635</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -20839,7 +20837,7 @@
         <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D83" s="1">
         <v>600</v>
@@ -20853,7 +20851,7 @@
         <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D84" s="1">
         <v>615</v>
@@ -20867,7 +20865,7 @@
         <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D85" s="1">
         <v>580</v>
@@ -20876,7 +20874,7 @@
         <v>570</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -20884,7 +20882,7 @@
         <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="D86" s="1">
         <v>640</v>
@@ -20899,7 +20897,7 @@
         <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="D87" s="1">
         <v>575</v>
@@ -20908,7 +20906,7 @@
         <v>570</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -20916,7 +20914,7 @@
         <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D88" s="1">
         <v>580</v>
@@ -20931,7 +20929,7 @@
         <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="D89" s="1">
         <v>690</v>
@@ -20940,7 +20938,7 @@
         <v>670</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -20948,7 +20946,7 @@
         <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="D90" s="1">
         <v>575</v>
@@ -20957,7 +20955,7 @@
         <v>570</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: update image oct-05
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/per-github/project-tennis/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF8CAB-E48D-1B40-8262-64D72DD15352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4612AD0B-1B8E-9849-B9DE-09301F270BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="25320" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5140" yWindow="760" windowWidth="28220" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -3272,9 +3272,6 @@
     <t>0903132099</t>
   </si>
   <si>
-    <t>Bé Chuột</t>
-  </si>
-  <si>
     <t>Ty Gia Long</t>
   </si>
   <si>
@@ -3288,9 +3285,6 @@
   </si>
   <si>
     <t>0913639634</t>
-  </si>
-  <si>
-    <t>Dũng Đầu Kéo</t>
   </si>
   <si>
     <t>Ngô Anh Đào</t>
@@ -6388,6 +6382,12 @@
   </si>
   <si>
     <t>Nam Sân Bay</t>
+  </si>
+  <si>
+    <t>Thanh Nhã ĐN</t>
+  </si>
+  <si>
+    <t>Dũng - Vận Tải - Việt Onion</t>
   </si>
 </sst>
 </file>
@@ -6816,8 +6816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I641"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A619" workbookViewId="0">
-      <selection activeCell="E639" sqref="E639"/>
+    <sheetView tabSelected="1" topLeftCell="A539" workbookViewId="0">
+      <selection activeCell="C581" sqref="C581"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6998,10 +6998,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="D10" s="7">
         <v>600</v>
@@ -7094,7 +7094,7 @@
         <v>9</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="D14" s="7">
         <v>650</v>
@@ -7201,7 +7201,7 @@
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="D19" s="12">
         <v>635</v>
@@ -7225,7 +7225,7 @@
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="D20" s="12">
         <v>640</v>
@@ -7249,7 +7249,7 @@
       </c>
       <c r="B21" s="11"/>
       <c r="C21" s="11" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="D21" s="12">
         <v>630</v>
@@ -7275,7 +7275,7 @@
       </c>
       <c r="B22" s="11"/>
       <c r="C22" s="11" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="D22" s="12">
         <v>635</v>
@@ -7296,10 +7296,10 @@
         <v>18</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="D23" s="12">
         <v>640</v>
@@ -7321,7 +7321,7 @@
       </c>
       <c r="B24" s="11"/>
       <c r="C24" s="11" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="D24" s="12">
         <v>650</v>
@@ -7365,7 +7365,7 @@
         <v>21</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="D26" s="22">
         <v>640</v>
@@ -7454,7 +7454,7 @@
       </c>
       <c r="B30" s="11"/>
       <c r="C30" s="11" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="D30" s="12">
         <v>605</v>
@@ -7564,7 +7564,7 @@
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="D35" s="12">
         <v>610</v>
@@ -7586,7 +7586,7 @@
         <v>31</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="D36" s="5">
         <v>605</v>
@@ -7607,7 +7607,7 @@
       </c>
       <c r="B37" s="11"/>
       <c r="C37" s="11" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="D37" s="12">
         <v>665</v>
@@ -7627,7 +7627,7 @@
         <v>33</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="D38" s="7">
         <v>615</v>
@@ -7686,7 +7686,7 @@
       </c>
       <c r="B41" s="11"/>
       <c r="C41" s="11" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="D41" s="12">
         <v>600</v>
@@ -7709,7 +7709,7 @@
       </c>
       <c r="B42" s="11"/>
       <c r="C42" s="11" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="D42" s="12">
         <v>650</v>
@@ -7751,7 +7751,7 @@
       </c>
       <c r="B44" s="11"/>
       <c r="C44" s="11" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="D44" s="12">
         <v>630</v>
@@ -7972,7 +7972,7 @@
       </c>
       <c r="B55" s="11"/>
       <c r="C55" s="11" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="D55" s="12">
         <v>625</v>
@@ -7993,7 +7993,7 @@
       </c>
       <c r="B56" s="11"/>
       <c r="C56" s="11" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D56" s="12">
         <v>610</v>
@@ -8030,7 +8030,7 @@
         <v>53</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="D58" s="5">
         <v>650</v>
@@ -8045,7 +8045,7 @@
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="11" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D59" s="12">
         <v>600</v>
@@ -8086,10 +8086,10 @@
         <v>56</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="D61" s="12">
         <v>625</v>
@@ -8110,7 +8110,7 @@
       </c>
       <c r="B62" s="11"/>
       <c r="C62" s="11" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="D62" s="12">
         <v>630</v>
@@ -8205,10 +8205,10 @@
         <v>62</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="D67" s="12">
         <v>615</v>
@@ -8245,10 +8245,10 @@
         <v>64</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="D69" s="12">
         <v>600</v>
@@ -8269,7 +8269,7 @@
       </c>
       <c r="B70" s="11"/>
       <c r="C70" s="11" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="D70" s="12">
         <v>605</v>
@@ -8396,7 +8396,7 @@
       </c>
       <c r="B76" s="11"/>
       <c r="C76" s="11" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="D76" s="12">
         <v>660</v>
@@ -8480,7 +8480,7 @@
       </c>
       <c r="B80" s="11"/>
       <c r="C80" s="11" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="D80" s="12">
         <v>600</v>
@@ -8526,7 +8526,7 @@
       </c>
       <c r="B82" s="11"/>
       <c r="C82" s="11" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="D82" s="12">
         <v>670</v>
@@ -8570,7 +8570,7 @@
       </c>
       <c r="B84" s="11"/>
       <c r="C84" s="11" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="D84" s="12">
         <v>615</v>
@@ -8589,7 +8589,7 @@
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="11" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="D85" s="12">
         <v>635</v>
@@ -8608,7 +8608,7 @@
       </c>
       <c r="B86" s="11"/>
       <c r="C86" s="11" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="D86" s="12">
         <v>690</v>
@@ -8631,7 +8631,7 @@
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="11" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="D87" s="12">
         <v>610</v>
@@ -8740,7 +8740,7 @@
       </c>
       <c r="B92" s="11"/>
       <c r="C92" s="11" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="D92" s="12">
         <v>655</v>
@@ -8760,10 +8760,10 @@
         <v>88</v>
       </c>
       <c r="B93" s="11" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="D93" s="12">
         <v>605</v>
@@ -8860,7 +8860,7 @@
       </c>
       <c r="B98" s="11"/>
       <c r="C98" s="11" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="D98" s="12">
         <v>645</v>
@@ -8988,7 +8988,7 @@
       </c>
       <c r="B104" s="11"/>
       <c r="C104" s="11" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="D104" s="12">
         <v>630</v>
@@ -9032,7 +9032,7 @@
       </c>
       <c r="B106" s="11"/>
       <c r="C106" s="11" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="D106" s="12">
         <v>660</v>
@@ -9052,7 +9052,7 @@
         <v>102</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="D107" s="7">
         <v>605</v>
@@ -9116,7 +9116,7 @@
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="11" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="D110" s="12">
         <v>600</v>
@@ -9135,7 +9135,7 @@
       </c>
       <c r="B111" s="11"/>
       <c r="C111" s="11" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="D111" s="12">
         <v>625</v>
@@ -9213,7 +9213,7 @@
       </c>
       <c r="B115" s="11"/>
       <c r="C115" s="11" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="D115" s="12">
         <v>600</v>
@@ -9234,7 +9234,7 @@
       </c>
       <c r="B116" s="11"/>
       <c r="C116" s="11" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="D116" s="12">
         <v>675</v>
@@ -9274,7 +9274,7 @@
       </c>
       <c r="B118" s="11"/>
       <c r="C118" s="11" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="D118" s="12">
         <v>675</v>
@@ -9293,7 +9293,7 @@
       </c>
       <c r="B119" s="11"/>
       <c r="C119" s="11" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D119" s="12">
         <v>600</v>
@@ -9316,7 +9316,7 @@
       </c>
       <c r="B120" s="11"/>
       <c r="C120" s="11" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="D120" s="12">
         <v>600</v>
@@ -9360,7 +9360,7 @@
       </c>
       <c r="B122" s="11"/>
       <c r="C122" s="11" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="D122" s="12">
         <v>645</v>
@@ -9383,7 +9383,7 @@
       </c>
       <c r="B123" s="11"/>
       <c r="C123" s="11" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="D123" s="12">
         <v>590</v>
@@ -9402,7 +9402,7 @@
       </c>
       <c r="B124" s="11"/>
       <c r="C124" s="11" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="D124" s="12">
         <v>615</v>
@@ -9421,7 +9421,7 @@
       </c>
       <c r="B125" s="11"/>
       <c r="C125" s="11" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="D125" s="12">
         <v>635</v>
@@ -9483,7 +9483,7 @@
         <v>123</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="D128" s="5">
         <v>635</v>
@@ -9501,7 +9501,7 @@
       </c>
       <c r="B129" s="11"/>
       <c r="C129" s="11" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="D129" s="12">
         <v>610</v>
@@ -9539,7 +9539,7 @@
       </c>
       <c r="B131" s="11"/>
       <c r="C131" s="11" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D131" s="12">
         <v>680</v>
@@ -9558,7 +9558,7 @@
       </c>
       <c r="B132" s="11"/>
       <c r="C132" s="11" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="D132" s="12">
         <v>590</v>
@@ -9600,7 +9600,7 @@
       </c>
       <c r="B134" s="11"/>
       <c r="C134" s="11" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="D134" s="12">
         <v>635</v>
@@ -9621,7 +9621,7 @@
       </c>
       <c r="B135" s="11"/>
       <c r="C135" s="11" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="D135" s="12">
         <v>610</v>
@@ -9738,7 +9738,7 @@
         <v>136</v>
       </c>
       <c r="C141" s="6" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D141" s="7">
         <v>765</v>
@@ -9756,7 +9756,7 @@
       </c>
       <c r="B142" s="11"/>
       <c r="C142" s="11" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="D142" s="12">
         <v>785</v>
@@ -9794,7 +9794,7 @@
       </c>
       <c r="B144" s="11"/>
       <c r="C144" s="11" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="D144" s="12">
         <v>985</v>
@@ -9834,7 +9834,7 @@
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="11" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="D146" s="12">
         <v>850</v>
@@ -9872,7 +9872,7 @@
       </c>
       <c r="B148" s="11"/>
       <c r="C148" s="11" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D148" s="12">
         <v>790</v>
@@ -9890,7 +9890,7 @@
         <v>144</v>
       </c>
       <c r="C149" s="6" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D149" s="7">
         <v>760</v>
@@ -9945,7 +9945,7 @@
       </c>
       <c r="B152" s="11"/>
       <c r="C152" s="11" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="D152" s="12">
         <v>840</v>
@@ -9966,7 +9966,7 @@
       </c>
       <c r="B153" s="11"/>
       <c r="C153" s="11" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="D153" s="12">
         <v>785</v>
@@ -9985,7 +9985,7 @@
       </c>
       <c r="B154" s="11"/>
       <c r="C154" s="11" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D154" s="12">
         <v>880</v>
@@ -10025,7 +10025,7 @@
       </c>
       <c r="B156" s="11"/>
       <c r="C156" s="11" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="D156" s="12">
         <v>830</v>
@@ -10046,7 +10046,7 @@
       </c>
       <c r="B157" s="11"/>
       <c r="C157" s="11" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="D157" s="12">
         <v>935</v>
@@ -10105,7 +10105,7 @@
       </c>
       <c r="B160" s="11"/>
       <c r="C160" s="11" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D160" s="12">
         <v>920</v>
@@ -10164,7 +10164,7 @@
       </c>
       <c r="B163" s="11"/>
       <c r="C163" s="11" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="D163" s="12">
         <v>810</v>
@@ -10185,7 +10185,7 @@
       </c>
       <c r="B164" s="11"/>
       <c r="C164" s="11" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="D164" s="12">
         <v>755</v>
@@ -10206,7 +10206,7 @@
       </c>
       <c r="B165" s="11"/>
       <c r="C165" s="11" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D165" s="12">
         <v>605</v>
@@ -10225,7 +10225,7 @@
       </c>
       <c r="B166" s="11"/>
       <c r="C166" s="11" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D166" s="12">
         <v>990</v>
@@ -10264,7 +10264,7 @@
         <v>163</v>
       </c>
       <c r="C168" s="6" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="D168" s="7">
         <v>735</v>
@@ -10282,7 +10282,7 @@
       </c>
       <c r="B169" s="11"/>
       <c r="C169" s="11" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="D169" s="12">
         <v>630</v>
@@ -10324,7 +10324,7 @@
       </c>
       <c r="B171" s="11"/>
       <c r="C171" s="11" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D171" s="12">
         <v>750</v>
@@ -10406,7 +10406,7 @@
       </c>
       <c r="B175" s="11"/>
       <c r="C175" s="11" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D175" s="12">
         <v>910</v>
@@ -10446,7 +10446,7 @@
       </c>
       <c r="B177" s="11"/>
       <c r="C177" s="11" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D177" s="12">
         <v>930</v>
@@ -10467,7 +10467,7 @@
       </c>
       <c r="B178" s="11"/>
       <c r="C178" s="11" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D178" s="12">
         <v>955</v>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="B179" s="11"/>
       <c r="C179" s="11" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="D179" s="12">
         <v>1010</v>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="B180" s="11"/>
       <c r="C180" s="11" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="D180" s="12">
         <v>670</v>
@@ -10549,7 +10549,7 @@
       </c>
       <c r="B182" s="11"/>
       <c r="C182" s="11" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="D182" s="12">
         <v>890</v>
@@ -10568,7 +10568,7 @@
       </c>
       <c r="B183" s="11"/>
       <c r="C183" s="11" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="D183" s="12">
         <v>815</v>
@@ -10587,7 +10587,7 @@
       </c>
       <c r="B184" s="11"/>
       <c r="C184" s="11" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D184" s="12">
         <v>835</v>
@@ -10608,7 +10608,7 @@
       </c>
       <c r="B185" s="11"/>
       <c r="C185" s="11" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D185" s="12">
         <v>735</v>
@@ -10629,7 +10629,7 @@
       </c>
       <c r="B186" s="11"/>
       <c r="C186" s="11" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="D186" s="12">
         <v>780</v>
@@ -10648,7 +10648,7 @@
       </c>
       <c r="B187" s="11"/>
       <c r="C187" s="11" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="D187" s="12">
         <v>810</v>
@@ -10667,7 +10667,7 @@
       </c>
       <c r="B188" s="11"/>
       <c r="C188" s="11" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="D188" s="12">
         <v>880</v>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="B189" s="11"/>
       <c r="C189" s="11" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="D189" s="12">
         <v>885</v>
@@ -10708,7 +10708,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="6" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D190" s="7">
         <v>695</v>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="B192" s="11"/>
       <c r="C192" s="11" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="D192" s="12">
         <v>880</v>
@@ -10763,7 +10763,7 @@
       </c>
       <c r="B193" s="11"/>
       <c r="C193" s="11" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D193" s="12">
         <v>745</v>
@@ -10822,7 +10822,7 @@
       </c>
       <c r="B196" s="11"/>
       <c r="C196" s="11" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="D196" s="12">
         <v>790</v>
@@ -10858,7 +10858,7 @@
       </c>
       <c r="B198" s="11"/>
       <c r="C198" s="11" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="D198" s="12">
         <v>740</v>
@@ -10877,7 +10877,7 @@
       </c>
       <c r="B199" s="11"/>
       <c r="C199" s="11" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="D199" s="12">
         <v>730</v>
@@ -10896,7 +10896,7 @@
       </c>
       <c r="B200" s="11"/>
       <c r="C200" s="11" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D200" s="12">
         <v>745</v>
@@ -10929,7 +10929,7 @@
       </c>
       <c r="B202" s="11"/>
       <c r="C202" s="11" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D202" s="12">
         <v>660</v>
@@ -11006,7 +11006,7 @@
         <v>201</v>
       </c>
       <c r="C206" s="6" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="D206" s="7">
         <v>690</v>
@@ -11040,7 +11040,7 @@
       </c>
       <c r="B208" s="11"/>
       <c r="C208" s="11" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D208" s="12">
         <v>760</v>
@@ -11059,7 +11059,7 @@
       </c>
       <c r="B209" s="11"/>
       <c r="C209" s="11" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D209" s="12">
         <v>725</v>
@@ -12091,7 +12091,7 @@
       </c>
       <c r="B256" s="11"/>
       <c r="C256" s="11" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="D256" s="12">
         <v>645</v>
@@ -15468,7 +15468,7 @@
       </c>
       <c r="F423" s="11"/>
       <c r="G423" s="11" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="H423" s="11"/>
       <c r="I423" s="11"/>
@@ -15626,7 +15626,7 @@
         <v>595</v>
       </c>
       <c r="F431" s="10" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="432" spans="1:9" x14ac:dyDescent="0.2">
@@ -16155,7 +16155,7 @@
         <v>716</v>
       </c>
       <c r="C458" s="11" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D458" s="12">
         <v>640</v>
@@ -16231,7 +16231,7 @@
       </c>
       <c r="B462" s="11"/>
       <c r="C462" s="11" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="D462" s="12">
         <v>615</v>
@@ -16240,7 +16240,7 @@
         <v>615</v>
       </c>
       <c r="F462" s="16" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="G462" s="11"/>
       <c r="H462" s="11"/>
@@ -17646,7 +17646,7 @@
       </c>
       <c r="B534" s="11"/>
       <c r="C534" s="11" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D534" s="12">
         <v>760</v>
@@ -17903,7 +17903,7 @@
       </c>
       <c r="B547" s="11"/>
       <c r="C547" s="11" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="D547" s="12">
         <v>670</v>
@@ -18002,7 +18002,7 @@
       </c>
       <c r="B552" s="11"/>
       <c r="C552" s="11" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D552" s="12">
         <v>700</v>
@@ -18155,7 +18155,7 @@
       </c>
       <c r="B560" s="11"/>
       <c r="C560" s="11" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="D560" s="12">
         <v>775</v>
@@ -18491,7 +18491,7 @@
       </c>
       <c r="B577" s="11"/>
       <c r="C577" s="11" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D577" s="12">
         <v>675</v>
@@ -18500,7 +18500,7 @@
         <v>665</v>
       </c>
       <c r="F577" s="16" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G577" s="11"/>
       <c r="H577" s="11"/>
@@ -18511,7 +18511,7 @@
         <v>575</v>
       </c>
       <c r="C578" s="6" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D578" s="7">
         <v>585</v>
@@ -18526,7 +18526,7 @@
       </c>
       <c r="B579" s="11"/>
       <c r="C579" s="11" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D579" s="12">
         <v>580</v>
@@ -18545,7 +18545,7 @@
       </c>
       <c r="B580" s="11"/>
       <c r="C580" s="11" t="s">
-        <v>918</v>
+        <v>1142</v>
       </c>
       <c r="D580" s="12">
         <v>580</v>
@@ -18564,7 +18564,7 @@
       </c>
       <c r="B581" s="11"/>
       <c r="C581" s="11" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="D581" s="12">
         <v>580</v>
@@ -18573,7 +18573,7 @@
         <v>580</v>
       </c>
       <c r="F581" s="16" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G581" s="11"/>
       <c r="H581" s="11"/>
@@ -18585,7 +18585,7 @@
       </c>
       <c r="B582" s="11"/>
       <c r="C582" s="11" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D582" s="12">
         <v>635</v>
@@ -18604,7 +18604,7 @@
       </c>
       <c r="B583" s="11"/>
       <c r="C583" s="11" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="D583" s="12">
         <v>610</v>
@@ -18613,7 +18613,7 @@
         <v>600</v>
       </c>
       <c r="F583" s="20" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="G583" s="11"/>
       <c r="H583" s="11"/>
@@ -18625,7 +18625,7 @@
       </c>
       <c r="B584" s="11"/>
       <c r="C584" s="11" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="D584" s="12">
         <v>605</v>
@@ -18634,11 +18634,11 @@
         <v>600</v>
       </c>
       <c r="F584" s="20" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="G584" s="11"/>
       <c r="H584" s="11" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="I584" s="11"/>
     </row>
@@ -18648,7 +18648,7 @@
       </c>
       <c r="B585" s="11"/>
       <c r="C585" s="11" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="D585" s="12">
         <v>690</v>
@@ -18666,7 +18666,7 @@
         <v>583</v>
       </c>
       <c r="C586" s="4" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="D586" s="5">
         <v>610</v>
@@ -18680,7 +18680,7 @@
         <v>584</v>
       </c>
       <c r="C587" s="11" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="D587" s="14">
         <v>600</v>
@@ -18694,7 +18694,7 @@
         <v>585</v>
       </c>
       <c r="C588" s="11" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="D588" s="14">
         <v>620</v>
@@ -18708,7 +18708,7 @@
         <v>586</v>
       </c>
       <c r="C589" s="11" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="D589" s="14">
         <v>620</v>
@@ -18722,7 +18722,7 @@
         <v>587</v>
       </c>
       <c r="C590" s="4" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="D590" s="5">
         <v>680</v>
@@ -18731,7 +18731,7 @@
         <v>670</v>
       </c>
       <c r="F590" s="10" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="591" spans="1:9" x14ac:dyDescent="0.2">
@@ -18739,7 +18739,7 @@
         <v>588</v>
       </c>
       <c r="C591" s="11" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D591" s="14">
         <v>745</v>
@@ -18753,7 +18753,7 @@
         <v>589</v>
       </c>
       <c r="C592" s="11" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D592" s="14">
         <v>725</v>
@@ -18762,7 +18762,7 @@
         <v>715</v>
       </c>
       <c r="F592" s="2" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="593" spans="1:6" x14ac:dyDescent="0.2">
@@ -18770,7 +18770,7 @@
         <v>590</v>
       </c>
       <c r="C593" s="11" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D593" s="14">
         <v>740</v>
@@ -18779,7 +18779,7 @@
         <v>730</v>
       </c>
       <c r="F593" s="2" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="594" spans="1:6" x14ac:dyDescent="0.2">
@@ -18787,7 +18787,7 @@
         <v>591</v>
       </c>
       <c r="C594" s="11" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="D594" s="14">
         <v>700</v>
@@ -18796,7 +18796,7 @@
         <v>690</v>
       </c>
       <c r="F594" s="2" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="595" spans="1:6" x14ac:dyDescent="0.2">
@@ -18804,7 +18804,7 @@
         <v>592</v>
       </c>
       <c r="C595" s="11" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D595" s="14">
         <v>750</v>
@@ -18813,7 +18813,7 @@
         <v>735</v>
       </c>
       <c r="F595" s="2" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="596" spans="1:6" x14ac:dyDescent="0.2">
@@ -18821,7 +18821,7 @@
         <v>593</v>
       </c>
       <c r="C596" s="11" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="D596" s="14">
         <v>600</v>
@@ -18830,7 +18830,7 @@
         <v>600</v>
       </c>
       <c r="F596" s="2" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="597" spans="1:6" x14ac:dyDescent="0.2">
@@ -18838,7 +18838,7 @@
         <v>594</v>
       </c>
       <c r="C597" s="11" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D597" s="14">
         <v>760</v>
@@ -18847,7 +18847,7 @@
         <v>750</v>
       </c>
       <c r="F597" s="2" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="598" spans="1:6" x14ac:dyDescent="0.2">
@@ -18855,7 +18855,7 @@
         <v>595</v>
       </c>
       <c r="C598" s="11" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D598" s="14">
         <v>600</v>
@@ -18864,7 +18864,7 @@
         <v>600</v>
       </c>
       <c r="F598" s="2" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="599" spans="1:6" x14ac:dyDescent="0.2">
@@ -18872,7 +18872,7 @@
         <v>597</v>
       </c>
       <c r="C599" s="11" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="D599" s="14">
         <v>720</v>
@@ -18881,7 +18881,7 @@
         <v>710</v>
       </c>
       <c r="F599" s="2" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="600" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -18889,7 +18889,7 @@
         <v>598</v>
       </c>
       <c r="C600" s="4" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D600" s="5">
         <v>655</v>
@@ -18906,7 +18906,7 @@
         <v>599</v>
       </c>
       <c r="C601" s="4" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D601" s="5">
         <v>750</v>
@@ -18920,7 +18920,7 @@
         <v>600</v>
       </c>
       <c r="C602" s="11" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="D602" s="14">
         <v>760</v>
@@ -18929,7 +18929,7 @@
         <v>740</v>
       </c>
       <c r="F602" s="2" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="603" spans="1:6" x14ac:dyDescent="0.2">
@@ -18937,7 +18937,7 @@
         <v>601</v>
       </c>
       <c r="C603" s="11" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="D603" s="14">
         <v>630</v>
@@ -18951,7 +18951,7 @@
         <v>602</v>
       </c>
       <c r="C604" s="11" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D604" s="14">
         <v>730</v>
@@ -18960,7 +18960,7 @@
         <v>715</v>
       </c>
       <c r="F604" s="2" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="605" spans="1:6" x14ac:dyDescent="0.2">
@@ -18968,7 +18968,7 @@
         <v>603</v>
       </c>
       <c r="C605" s="11" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="D605" s="14">
         <v>610</v>
@@ -18977,7 +18977,7 @@
         <v>600</v>
       </c>
       <c r="F605" s="2" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="606" spans="1:6" x14ac:dyDescent="0.2">
@@ -18985,7 +18985,7 @@
         <v>604</v>
       </c>
       <c r="C606" s="11" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="D606" s="14">
         <v>730</v>
@@ -18999,7 +18999,7 @@
         <v>605</v>
       </c>
       <c r="C607" s="4" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D607" s="5">
         <v>685</v>
@@ -19013,7 +19013,7 @@
         <v>606</v>
       </c>
       <c r="C608" s="11" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="D608" s="14">
         <v>625</v>
@@ -19022,7 +19022,7 @@
         <v>615</v>
       </c>
       <c r="F608" s="2" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="609" spans="1:6" x14ac:dyDescent="0.2">
@@ -19030,7 +19030,7 @@
         <v>607</v>
       </c>
       <c r="C609" s="11" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="D609" s="14">
         <v>645</v>
@@ -19039,7 +19039,7 @@
         <v>635</v>
       </c>
       <c r="F609" s="2" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="610" spans="1:6" x14ac:dyDescent="0.2">
@@ -19047,7 +19047,7 @@
         <v>608</v>
       </c>
       <c r="C610" s="11" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="D610" s="14">
         <v>600</v>
@@ -19061,7 +19061,7 @@
         <v>609</v>
       </c>
       <c r="C611" s="11" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="D611" s="14">
         <v>660</v>
@@ -19070,7 +19070,7 @@
         <v>655</v>
       </c>
       <c r="F611" s="2" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="612" spans="1:6" x14ac:dyDescent="0.2">
@@ -19078,7 +19078,7 @@
         <v>610</v>
       </c>
       <c r="C612" s="11" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="D612" s="14">
         <v>590</v>
@@ -19087,7 +19087,7 @@
         <v>590</v>
       </c>
       <c r="F612" s="2" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="613" spans="1:6" x14ac:dyDescent="0.2">
@@ -19095,7 +19095,7 @@
         <v>611</v>
       </c>
       <c r="C613" s="11" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="D613" s="14">
         <v>620</v>
@@ -19104,7 +19104,7 @@
         <v>600</v>
       </c>
       <c r="F613" s="2" t="s">
-        <v>1084</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="614" spans="1:6" x14ac:dyDescent="0.2">
@@ -19112,7 +19112,7 @@
         <v>612</v>
       </c>
       <c r="C614" s="11" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
       <c r="D614" s="14">
         <v>640</v>
@@ -19121,7 +19121,7 @@
         <v>630</v>
       </c>
       <c r="F614" s="2" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="615" spans="1:6" x14ac:dyDescent="0.2">
@@ -19129,7 +19129,7 @@
         <v>613</v>
       </c>
       <c r="C615" s="11" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="D615" s="14">
         <v>640</v>
@@ -19138,7 +19138,7 @@
         <v>630</v>
       </c>
       <c r="F615" s="2" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="616" spans="1:6" x14ac:dyDescent="0.2">
@@ -19146,7 +19146,7 @@
         <v>614</v>
       </c>
       <c r="C616" s="11" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
       <c r="D616" s="14">
         <v>640</v>
@@ -19160,7 +19160,7 @@
         <v>615</v>
       </c>
       <c r="C617" s="11" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
       <c r="D617" s="14">
         <v>615</v>
@@ -19169,7 +19169,7 @@
         <v>605</v>
       </c>
       <c r="F617" s="2" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="618" spans="1:6" x14ac:dyDescent="0.2">
@@ -19177,7 +19177,7 @@
         <v>616</v>
       </c>
       <c r="C618" s="11" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="D618" s="14">
         <v>625</v>
@@ -19191,7 +19191,7 @@
         <v>617</v>
       </c>
       <c r="C619" s="11" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
       <c r="D619" s="14">
         <v>625</v>
@@ -19205,7 +19205,7 @@
         <v>618</v>
       </c>
       <c r="C620" s="11" t="s">
-        <v>1094</v>
+        <v>1092</v>
       </c>
       <c r="D620" s="14">
         <v>600</v>
@@ -19214,7 +19214,7 @@
         <v>600</v>
       </c>
       <c r="F620" s="2" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="621" spans="1:6" x14ac:dyDescent="0.2">
@@ -19222,7 +19222,7 @@
         <v>619</v>
       </c>
       <c r="C621" s="11" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="D621" s="14">
         <v>625</v>
@@ -19236,7 +19236,7 @@
         <v>620</v>
       </c>
       <c r="C622" s="11" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="D622" s="14">
         <v>600</v>
@@ -19250,7 +19250,7 @@
         <v>621</v>
       </c>
       <c r="C623" s="11" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="D623" s="14">
         <v>610</v>
@@ -19259,7 +19259,7 @@
         <v>600</v>
       </c>
       <c r="F623" s="2" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="624" spans="1:6" x14ac:dyDescent="0.2">
@@ -19267,7 +19267,7 @@
         <v>622</v>
       </c>
       <c r="C624" s="11" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="D624" s="14">
         <v>635</v>
@@ -19276,7 +19276,7 @@
         <v>620</v>
       </c>
       <c r="F624" s="2" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="625" spans="1:6" x14ac:dyDescent="0.2">
@@ -19284,7 +19284,7 @@
         <v>623</v>
       </c>
       <c r="C625" s="11" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="D625" s="14">
         <v>600</v>
@@ -19298,7 +19298,7 @@
         <v>624</v>
       </c>
       <c r="C626" s="11" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="D626" s="14">
         <v>605</v>
@@ -19312,7 +19312,7 @@
         <v>625</v>
       </c>
       <c r="C627" s="11" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="D627" s="14">
         <v>635</v>
@@ -19326,7 +19326,7 @@
         <v>626</v>
       </c>
       <c r="C628" s="11" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="D628" s="14">
         <v>605</v>
@@ -19335,7 +19335,7 @@
         <v>600</v>
       </c>
       <c r="F628" s="2" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="629" spans="1:6" x14ac:dyDescent="0.2">
@@ -19343,7 +19343,7 @@
         <v>627</v>
       </c>
       <c r="C629" s="11" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="D629" s="14">
         <v>650</v>
@@ -19352,7 +19352,7 @@
         <v>640</v>
       </c>
       <c r="F629" s="2" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
     </row>
     <row r="630" spans="1:6" x14ac:dyDescent="0.2">
@@ -19360,7 +19360,7 @@
         <v>628</v>
       </c>
       <c r="C630" s="11" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="D630" s="14">
         <v>640</v>
@@ -19374,7 +19374,7 @@
         <v>629</v>
       </c>
       <c r="C631" s="11" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="D631" s="14">
         <v>600</v>
@@ -19388,7 +19388,7 @@
         <v>630</v>
       </c>
       <c r="C632" s="11" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="D632" s="14">
         <v>605</v>
@@ -19402,7 +19402,7 @@
         <v>631</v>
       </c>
       <c r="C633" s="11" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D633" s="14">
         <v>640</v>
@@ -19411,7 +19411,7 @@
         <v>635</v>
       </c>
       <c r="F633" s="2" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="634" spans="1:6" x14ac:dyDescent="0.2">
@@ -19419,7 +19419,7 @@
         <v>632</v>
       </c>
       <c r="C634" s="11" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="D634" s="14">
         <v>635</v>
@@ -19433,7 +19433,7 @@
         <v>633</v>
       </c>
       <c r="C635" s="11" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="D635" s="14">
         <v>600</v>
@@ -19447,7 +19447,7 @@
         <v>634</v>
       </c>
       <c r="C636" s="11" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="D636" s="14">
         <v>605</v>
@@ -19456,7 +19456,7 @@
         <v>600</v>
       </c>
       <c r="F636" s="2" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.2">
@@ -19464,7 +19464,7 @@
         <v>635</v>
       </c>
       <c r="C637" s="11" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="D637" s="14">
         <v>630</v>
@@ -19473,7 +19473,7 @@
         <v>620</v>
       </c>
       <c r="F637" s="2" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="638" spans="1:6" x14ac:dyDescent="0.2">
@@ -19481,7 +19481,7 @@
         <v>636</v>
       </c>
       <c r="C638" s="11" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D638" s="14">
         <v>620</v>
@@ -19490,7 +19490,7 @@
         <v>610</v>
       </c>
       <c r="F638" s="2" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="639" spans="1:6" x14ac:dyDescent="0.2">
@@ -19498,7 +19498,7 @@
         <v>637</v>
       </c>
       <c r="C639" s="11" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D639" s="14">
         <v>625</v>
@@ -19512,7 +19512,7 @@
         <v>638</v>
       </c>
       <c r="C640" s="11" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="D640" s="14">
         <v>680</v>
@@ -19526,13 +19526,13 @@
         <v>639</v>
       </c>
       <c r="C641" s="11" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="D641" s="14">
         <v>625</v>
       </c>
       <c r="E641" s="1">
-        <v>625</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>
@@ -19550,8 +19550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A50" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19649,7 +19649,7 @@
         <v>560</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -19687,7 +19687,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="D9" s="22">
         <v>635</v>
@@ -19807,7 +19807,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="D17" s="7">
         <v>690</v>
@@ -19824,7 +19824,7 @@
         <v>13</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="D18" s="5">
         <v>675</v>
@@ -20759,7 +20759,7 @@
         <v>73</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>912</v>
+        <v>1141</v>
       </c>
       <c r="D78" s="12">
         <v>635</v>
@@ -20773,7 +20773,7 @@
         <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D79" s="1">
         <v>700</v>
@@ -20788,7 +20788,7 @@
         <v>75</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="D80" s="7">
         <v>680</v>
@@ -20803,7 +20803,7 @@
         <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="D81" s="1">
         <v>620</v>
@@ -20812,7 +20812,7 @@
         <v>610</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
@@ -20820,7 +20820,7 @@
         <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="D82" s="1">
         <v>645</v>
@@ -20829,7 +20829,7 @@
         <v>635</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -20837,7 +20837,7 @@
         <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="D83" s="1">
         <v>600</v>
@@ -20851,7 +20851,7 @@
         <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="D84" s="1">
         <v>615</v>
@@ -20865,7 +20865,7 @@
         <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="D85" s="1">
         <v>580</v>
@@ -20874,7 +20874,7 @@
         <v>570</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -20882,7 +20882,7 @@
         <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="D86" s="1">
         <v>640</v>
@@ -20897,7 +20897,7 @@
         <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="D87" s="1">
         <v>575</v>
@@ -20906,7 +20906,7 @@
         <v>570</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
@@ -20914,7 +20914,7 @@
         <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="D88" s="1">
         <v>580</v>
@@ -20929,7 +20929,7 @@
         <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="D89" s="1">
         <v>690</v>
@@ -20938,7 +20938,7 @@
         <v>670</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -20946,7 +20946,7 @@
         <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="D90" s="1">
         <v>575</v>
@@ -20955,7 +20955,7 @@
         <v>570</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
chore: update score apr 3
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,20 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{914D047E-E3F0-904C-914F-9B614DBAE5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD7FAFED-218C-BC4B-A3F2-8557017D2A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15280" yWindow="760" windowWidth="17980" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19700" yWindow="500" windowWidth="17980" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
     <sheet name="Nữ " sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="1281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1434" uniqueCount="1282">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -6751,6 +6764,9 @@
   </si>
   <si>
     <t>610</t>
+  </si>
+  <si>
+    <t>Huân 276</t>
   </si>
 </sst>
 </file>
@@ -7151,6 +7167,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7167,10 +7187,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8334,8 +8350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A661" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E714"/>
+    <sheetView showGridLines="0" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C715"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8355,17 +8371,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
       <c r="J1" s="28"/>
       <c r="K1" s="31"/>
       <c r="L1" s="31"/>
@@ -8385,17 +8401,17 @@
       <c r="Z1" s="31"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
       <c r="J2" s="28"/>
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
@@ -8452,10 +8468,10 @@
       <c r="C4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="80"/>
+      <c r="E4" s="82"/>
       <c r="F4" s="34" t="s">
         <v>6</v>
       </c>
@@ -11669,7 +11685,7 @@
         <v>131</v>
       </c>
       <c r="D87" s="44">
-        <v>645</v>
+        <v>635</v>
       </c>
       <c r="E87" s="44">
         <v>625</v>
@@ -12515,7 +12531,7 @@
         <v>1080</v>
       </c>
       <c r="D109" s="44">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="E109" s="44">
         <v>700</v>
@@ -12627,7 +12643,7 @@
         <v>1082</v>
       </c>
       <c r="D112" s="44">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="E112" s="44">
         <v>700</v>
@@ -35149,11 +35165,19 @@
       <c r="Z714" s="31"/>
     </row>
     <row r="715" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A715" s="28"/>
-      <c r="B715" s="28"/>
-      <c r="C715" s="28"/>
-      <c r="D715" s="33"/>
-      <c r="E715" s="33"/>
+      <c r="A715" s="54">
+        <v>710</v>
+      </c>
+      <c r="B715" s="54"/>
+      <c r="C715" s="54" t="s">
+        <v>1281</v>
+      </c>
+      <c r="D715" s="55">
+        <v>600</v>
+      </c>
+      <c r="E715" s="55">
+        <v>600</v>
+      </c>
       <c r="F715" s="28"/>
       <c r="G715" s="28"/>
       <c r="H715" s="28"/>
@@ -43174,7 +43198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A77" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" workbookViewId="0">
       <selection activeCell="E105" sqref="D6:E105"/>
     </sheetView>
   </sheetViews>
@@ -43195,17 +43219,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
       <c r="J1" s="3"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -43225,17 +43249,17 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
       <c r="J2" s="3"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
@@ -43292,10 +43316,10 @@
       <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="81" t="s">
+      <c r="D4" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="83"/>
+      <c r="E4" s="85"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -46950,7 +46974,7 @@
       <c r="Y102" s="4"/>
       <c r="Z102" s="4"/>
     </row>
-    <row r="103" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:26" s="77" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="54">
         <v>98</v>
       </c>
@@ -46986,7 +47010,7 @@
       <c r="Y103" s="69"/>
       <c r="Z103" s="69"/>
     </row>
-    <row r="104" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26" s="77" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="54">
         <v>99</v>
       </c>
@@ -47000,7 +47024,7 @@
       <c r="E104" s="55">
         <v>590</v>
       </c>
-      <c r="F104" s="85" t="s">
+      <c r="F104" s="78" t="s">
         <v>1231</v>
       </c>
       <c r="G104" s="54"/>
@@ -47024,7 +47048,7 @@
       <c r="Y104" s="69"/>
       <c r="Z104" s="69"/>
     </row>
-    <row r="105" spans="1:26" s="84" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:26" s="77" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="54">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
chore: update score on apr 22
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F603A74-0012-C54D-BCB7-9743E622506C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CE5937-383B-864C-B969-916CF220BBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15600" yWindow="760" windowWidth="18960" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15600" yWindow="760" windowWidth="18960" windowHeight="20300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nam" sheetId="1" r:id="rId1"/>
@@ -5309,8 +5309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A85" zoomScale="87" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView showGridLines="0" topLeftCell="A689" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E715"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -16954,10 +16954,10 @@
         <v>400</v>
       </c>
       <c r="D313" s="2">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="E313" s="2">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="F313" s="22"/>
       <c r="G313" s="23"/>
@@ -39841,8 +39841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:E105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
chore: update score on one yr anniversay
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CE5937-383B-864C-B969-916CF220BBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E5F84B-5C3A-0240-BA9A-D152AB3FDD0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15600" yWindow="760" windowWidth="18960" windowHeight="20300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1281" uniqueCount="1237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="1272">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -3745,13 +3745,118 @@
   </si>
   <si>
     <t>0918151894</t>
+  </si>
+  <si>
+    <t>Phú HT</t>
+  </si>
+  <si>
+    <t>Vương LV</t>
+  </si>
+  <si>
+    <t>Cường Phú Nhuận</t>
+  </si>
+  <si>
+    <t>Gia Khánh</t>
+  </si>
+  <si>
+    <t>Hùng Tam Kỳ</t>
+  </si>
+  <si>
+    <t>Johnny Cường</t>
+  </si>
+  <si>
+    <t>Henry Trường</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mẫn Seven </t>
+  </si>
+  <si>
+    <t>Được Hải Sản</t>
+  </si>
+  <si>
+    <t>Thiên Thới An</t>
+  </si>
+  <si>
+    <t>Vị Thới An</t>
+  </si>
+  <si>
+    <t>Xuân Chính Thắng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bảo Thép </t>
+  </si>
+  <si>
+    <t>Anh Võ Thép</t>
+  </si>
+  <si>
+    <t>Phương Toa Xe</t>
+  </si>
+  <si>
+    <t>Hòa Toa Xe</t>
+  </si>
+  <si>
+    <t>Vũ Vsip</t>
+  </si>
+  <si>
+    <t>Sơn Quỹ Tín Dụng NCT</t>
+  </si>
+  <si>
+    <t>Thái Tuấn Kiều</t>
+  </si>
+  <si>
+    <t>Phong 555</t>
+  </si>
+  <si>
+    <t>Bình Thới An</t>
+  </si>
+  <si>
+    <t>Phúc Thới An</t>
+  </si>
+  <si>
+    <t>Trí Gildden</t>
+  </si>
+  <si>
+    <t>Giải Chính Thắng</t>
+  </si>
+  <si>
+    <t>Lợi Q10</t>
+  </si>
+  <si>
+    <t>Hải VIB</t>
+  </si>
+  <si>
+    <t>Khánh Head</t>
+  </si>
+  <si>
+    <t>Vũ Quảng Ngãi</t>
+  </si>
+  <si>
+    <t>Giá Thủ Đức</t>
+  </si>
+  <si>
+    <t>Tú Gò Vấp</t>
+  </si>
+  <si>
+    <t>Minitao</t>
+  </si>
+  <si>
+    <t>Bình Củ Chi</t>
+  </si>
+  <si>
+    <t>Cường Tâm Linh</t>
+  </si>
+  <si>
+    <t>Tân Phú Yên</t>
+  </si>
+  <si>
+    <t>Ly Yoga</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -3809,6 +3914,36 @@
     <font>
       <sz val="11"/>
       <color indexed="15"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -4009,7 +4144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4147,6 +4282,38 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5309,8 +5476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A689" zoomScale="87" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E715"/>
+    <sheetView showGridLines="0" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B749" sqref="B749"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6220,13 +6387,13 @@
         <v>20</v>
       </c>
       <c r="B25" s="22"/>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="80" t="s">
         <v>37</v>
       </c>
-      <c r="D25" s="2">
-        <v>640</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="81">
+        <v>635</v>
+      </c>
+      <c r="E25" s="81">
         <v>630</v>
       </c>
       <c r="F25" s="1" t="s">
@@ -6258,13 +6425,13 @@
         <v>21</v>
       </c>
       <c r="B26" s="28"/>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="80" t="s">
         <v>1132</v>
       </c>
-      <c r="D26" s="2">
-        <v>650</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="81">
+        <v>645</v>
+      </c>
+      <c r="E26" s="81">
         <v>630</v>
       </c>
       <c r="F26" s="28"/>
@@ -7438,13 +7605,13 @@
         <v>53</v>
       </c>
       <c r="B58" s="22"/>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="82" t="s">
         <v>1141</v>
       </c>
-      <c r="D58" s="2">
-        <v>650</v>
-      </c>
-      <c r="E58" s="2">
+      <c r="D58" s="83">
+        <v>665</v>
+      </c>
+      <c r="E58" s="83">
         <v>645</v>
       </c>
       <c r="F58" s="22"/>
@@ -7666,14 +7833,14 @@
       <c r="B64" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="C64" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="D64" s="2">
-        <v>640</v>
-      </c>
-      <c r="E64" s="2">
-        <v>630</v>
+      <c r="D64" s="81">
+        <v>635</v>
+      </c>
+      <c r="E64" s="81">
+        <v>625</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>80</v>
@@ -7778,13 +7945,13 @@
       <c r="B67" s="1" t="s">
         <v>1144</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C67" s="82" t="s">
         <v>1144</v>
       </c>
-      <c r="D67" s="2">
-        <v>615</v>
-      </c>
-      <c r="E67" s="2">
+      <c r="D67" s="83">
+        <v>620</v>
+      </c>
+      <c r="E67" s="83">
         <v>615</v>
       </c>
       <c r="F67" s="22"/>
@@ -8524,13 +8691,13 @@
         <v>82</v>
       </c>
       <c r="B87" s="22"/>
-      <c r="C87" s="1" t="s">
+      <c r="C87" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="D87" s="2">
-        <v>635</v>
-      </c>
-      <c r="E87" s="2">
+      <c r="D87" s="83">
+        <v>650</v>
+      </c>
+      <c r="E87" s="83">
         <v>625</v>
       </c>
       <c r="F87" s="1" t="s">
@@ -8824,13 +8991,13 @@
         <v>90</v>
       </c>
       <c r="B95" s="22"/>
-      <c r="C95" s="1" t="s">
+      <c r="C95" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="D95" s="2">
-        <v>615</v>
-      </c>
-      <c r="E95" s="2">
+      <c r="D95" s="81">
+        <v>610</v>
+      </c>
+      <c r="E95" s="81">
         <v>610</v>
       </c>
       <c r="F95" s="22"/>
@@ -9260,13 +9427,13 @@
         <v>102</v>
       </c>
       <c r="B107" s="22"/>
-      <c r="C107" s="1" t="s">
+      <c r="C107" s="80" t="s">
         <v>1157</v>
       </c>
-      <c r="D107" s="2">
-        <v>605</v>
-      </c>
-      <c r="E107" s="2">
+      <c r="D107" s="81">
+        <v>600</v>
+      </c>
+      <c r="E107" s="81">
         <v>600</v>
       </c>
       <c r="F107" s="22"/>
@@ -9296,13 +9463,13 @@
         <v>103</v>
       </c>
       <c r="B108" s="22"/>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="80" t="s">
         <v>130</v>
       </c>
-      <c r="D108" s="2">
-        <v>670</v>
-      </c>
-      <c r="E108" s="2">
+      <c r="D108" s="81">
+        <v>665</v>
+      </c>
+      <c r="E108" s="81">
         <v>640</v>
       </c>
       <c r="F108" s="1" t="s">
@@ -9334,13 +9501,13 @@
         <v>104</v>
       </c>
       <c r="B109" s="22"/>
-      <c r="C109" s="1" t="s">
+      <c r="C109" s="82" t="s">
         <v>1032</v>
       </c>
-      <c r="D109" s="2">
-        <v>720</v>
-      </c>
-      <c r="E109" s="2">
+      <c r="D109" s="83">
+        <v>735</v>
+      </c>
+      <c r="E109" s="83">
         <v>700</v>
       </c>
       <c r="F109" s="1" t="s">
@@ -9588,14 +9755,14 @@
         <v>111</v>
       </c>
       <c r="B116" s="22"/>
-      <c r="C116" s="1" t="s">
+      <c r="C116" s="80" t="s">
         <v>1161</v>
       </c>
-      <c r="D116" s="2">
-        <v>660</v>
-      </c>
-      <c r="E116" s="2">
-        <v>660</v>
+      <c r="D116" s="81">
+        <v>655</v>
+      </c>
+      <c r="E116" s="81">
+        <v>650</v>
       </c>
       <c r="F116" s="34" t="s">
         <v>1236</v>
@@ -9626,13 +9793,13 @@
         <v>112</v>
       </c>
       <c r="B117" s="22"/>
-      <c r="C117" s="1" t="s">
+      <c r="C117" s="82" t="s">
         <v>135</v>
       </c>
-      <c r="D117" s="2">
-        <v>585</v>
-      </c>
-      <c r="E117" s="2">
+      <c r="D117" s="83">
+        <v>590</v>
+      </c>
+      <c r="E117" s="83">
         <v>580</v>
       </c>
       <c r="F117" s="22"/>
@@ -10108,13 +10275,13 @@
         <v>125</v>
       </c>
       <c r="B130" s="22"/>
-      <c r="C130" s="1" t="s">
+      <c r="C130" s="82" t="s">
         <v>146</v>
       </c>
-      <c r="D130" s="2">
-        <v>660</v>
-      </c>
-      <c r="E130" s="2">
+      <c r="D130" s="83">
+        <v>675</v>
+      </c>
+      <c r="E130" s="83">
         <v>655</v>
       </c>
       <c r="F130" s="22"/>
@@ -10218,14 +10385,14 @@
         <v>128</v>
       </c>
       <c r="B133" s="22"/>
-      <c r="C133" s="1" t="s">
+      <c r="C133" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="D133" s="2">
-        <v>680</v>
-      </c>
-      <c r="E133" s="2">
+      <c r="D133" s="83">
         <v>685</v>
+      </c>
+      <c r="E133" s="83">
+        <v>670</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>149</v>
@@ -12526,13 +12693,13 @@
         <v>190</v>
       </c>
       <c r="B195" s="22"/>
-      <c r="C195" s="1" t="s">
+      <c r="C195" s="80" t="s">
         <v>210</v>
       </c>
-      <c r="D195" s="2">
-        <v>725</v>
-      </c>
-      <c r="E195" s="2">
+      <c r="D195" s="81">
+        <v>720</v>
+      </c>
+      <c r="E195" s="81">
         <v>700</v>
       </c>
       <c r="F195" s="22"/>
@@ -12780,14 +12947,14 @@
         <v>197</v>
       </c>
       <c r="B202" s="22"/>
-      <c r="C202" s="1" t="s">
+      <c r="C202" s="80" t="s">
         <v>1210</v>
       </c>
-      <c r="D202" s="2">
-        <v>650</v>
-      </c>
-      <c r="E202" s="2">
-        <v>640</v>
+      <c r="D202" s="81">
+        <v>645</v>
+      </c>
+      <c r="E202" s="81">
+        <v>635</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>215</v>
@@ -12962,14 +13129,14 @@
         <v>202</v>
       </c>
       <c r="B207" s="22"/>
-      <c r="C207" s="1" t="s">
+      <c r="C207" s="80" t="s">
         <v>219</v>
       </c>
-      <c r="D207" s="2">
-        <v>740</v>
-      </c>
-      <c r="E207" s="2">
-        <v>740</v>
+      <c r="D207" s="81">
+        <v>735</v>
+      </c>
+      <c r="E207" s="81">
+        <v>730</v>
       </c>
       <c r="F207" s="22"/>
       <c r="G207" s="23"/>
@@ -14222,14 +14389,14 @@
         <v>235</v>
       </c>
       <c r="B240" s="22"/>
-      <c r="C240" s="1" t="s">
+      <c r="C240" s="82" t="s">
         <v>285</v>
       </c>
-      <c r="D240" s="2">
-        <v>610</v>
-      </c>
-      <c r="E240" s="2">
-        <v>600</v>
+      <c r="D240" s="83">
+        <v>635</v>
+      </c>
+      <c r="E240" s="83">
+        <v>620</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>286</v>
@@ -14638,13 +14805,13 @@
         <v>246</v>
       </c>
       <c r="B251" s="22"/>
-      <c r="C251" s="1" t="s">
+      <c r="C251" s="84" t="s">
         <v>304</v>
       </c>
-      <c r="D251" s="2">
-        <v>645</v>
-      </c>
-      <c r="E251" s="2">
+      <c r="D251" s="85">
+        <v>655</v>
+      </c>
+      <c r="E251" s="85">
         <v>630</v>
       </c>
       <c r="F251" s="1" t="s">
@@ -14826,14 +14993,14 @@
         <v>251</v>
       </c>
       <c r="B256" s="22"/>
-      <c r="C256" s="1" t="s">
+      <c r="C256" s="80" t="s">
         <v>1061</v>
       </c>
-      <c r="D256" s="2">
-        <v>635</v>
-      </c>
-      <c r="E256" s="2">
-        <v>635</v>
+      <c r="D256" s="81">
+        <v>630</v>
+      </c>
+      <c r="E256" s="81">
+        <v>630</v>
       </c>
       <c r="F256" s="1" t="s">
         <v>313</v>
@@ -15422,14 +15589,14 @@
         <v>267</v>
       </c>
       <c r="B272" s="22"/>
-      <c r="C272" s="1" t="s">
+      <c r="C272" s="82" t="s">
         <v>338</v>
       </c>
-      <c r="D272" s="2">
-        <v>650</v>
-      </c>
-      <c r="E272" s="2">
-        <v>650</v>
+      <c r="D272" s="83">
+        <v>690</v>
+      </c>
+      <c r="E272" s="83">
+        <v>670</v>
       </c>
       <c r="F272" s="22"/>
       <c r="G272" s="23"/>
@@ -15610,13 +15777,13 @@
         <v>272</v>
       </c>
       <c r="B277" s="22"/>
-      <c r="C277" s="1" t="s">
+      <c r="C277" s="84" t="s">
         <v>347</v>
       </c>
-      <c r="D277" s="2">
-        <v>630</v>
-      </c>
-      <c r="E277" s="2">
+      <c r="D277" s="85">
+        <v>635</v>
+      </c>
+      <c r="E277" s="85">
         <v>610</v>
       </c>
       <c r="F277" s="1" t="s">
@@ -15648,14 +15815,14 @@
         <v>273</v>
       </c>
       <c r="B278" s="22"/>
-      <c r="C278" s="1" t="s">
+      <c r="C278" s="82" t="s">
         <v>349</v>
       </c>
-      <c r="D278" s="2">
-        <v>685</v>
-      </c>
-      <c r="E278" s="2">
-        <v>660</v>
+      <c r="D278" s="83">
+        <v>695</v>
+      </c>
+      <c r="E278" s="83">
+        <v>670</v>
       </c>
       <c r="F278" s="1" t="s">
         <v>350</v>
@@ -16058,13 +16225,13 @@
         <v>284</v>
       </c>
       <c r="B289" s="22"/>
-      <c r="C289" s="1" t="s">
+      <c r="C289" s="82" t="s">
         <v>364</v>
       </c>
-      <c r="D289" s="2">
-        <v>660</v>
-      </c>
-      <c r="E289" s="2">
+      <c r="D289" s="83">
+        <v>675</v>
+      </c>
+      <c r="E289" s="83">
         <v>650</v>
       </c>
       <c r="F289" s="1" t="s">
@@ -16362,13 +16529,13 @@
         <v>292</v>
       </c>
       <c r="B297" s="22"/>
-      <c r="C297" s="1" t="s">
+      <c r="C297" s="84" t="s">
         <v>378</v>
       </c>
-      <c r="D297" s="2">
-        <v>635</v>
-      </c>
-      <c r="E297" s="2">
+      <c r="D297" s="85">
+        <v>640</v>
+      </c>
+      <c r="E297" s="85">
         <v>615</v>
       </c>
       <c r="F297" s="1" t="s">
@@ -16512,14 +16679,14 @@
         <v>296</v>
       </c>
       <c r="B301" s="22"/>
-      <c r="C301" s="1" t="s">
+      <c r="C301" s="82" t="s">
         <v>385</v>
       </c>
-      <c r="D301" s="2">
-        <v>615</v>
-      </c>
-      <c r="E301" s="2">
-        <v>605</v>
+      <c r="D301" s="83">
+        <v>640</v>
+      </c>
+      <c r="E301" s="83">
+        <v>625</v>
       </c>
       <c r="F301" s="1" t="s">
         <v>386</v>
@@ -16804,13 +16971,13 @@
         <v>304</v>
       </c>
       <c r="B309" s="22"/>
-      <c r="C309" s="1" t="s">
+      <c r="C309" s="80" t="s">
         <v>395</v>
       </c>
-      <c r="D309" s="2">
-        <v>620</v>
-      </c>
-      <c r="E309" s="2">
+      <c r="D309" s="81">
+        <v>615</v>
+      </c>
+      <c r="E309" s="81">
         <v>605</v>
       </c>
       <c r="F309" s="1" t="s">
@@ -20332,14 +20499,14 @@
         <v>399</v>
       </c>
       <c r="B404" s="22"/>
-      <c r="C404" s="1" t="s">
+      <c r="C404" s="82" t="s">
         <v>537</v>
       </c>
-      <c r="D404" s="2">
+      <c r="D404" s="83">
+        <v>680</v>
+      </c>
+      <c r="E404" s="83">
         <v>670</v>
-      </c>
-      <c r="E404" s="2">
-        <v>650</v>
       </c>
       <c r="F404" s="1" t="s">
         <v>538</v>
@@ -20558,13 +20725,13 @@
         <v>405</v>
       </c>
       <c r="B410" s="22"/>
-      <c r="C410" s="1" t="s">
+      <c r="C410" s="82" t="s">
         <v>547</v>
       </c>
-      <c r="D410" s="2">
-        <v>740</v>
-      </c>
-      <c r="E410" s="2">
+      <c r="D410" s="83">
+        <v>745</v>
+      </c>
+      <c r="E410" s="83">
         <v>730</v>
       </c>
       <c r="F410" s="22"/>
@@ -20632,14 +20799,14 @@
         <v>407</v>
       </c>
       <c r="B412" s="22"/>
-      <c r="C412" s="1" t="s">
+      <c r="C412" s="80" t="s">
         <v>550</v>
       </c>
-      <c r="D412" s="2">
-        <v>675</v>
-      </c>
-      <c r="E412" s="2">
+      <c r="D412" s="81">
         <v>670</v>
+      </c>
+      <c r="E412" s="81">
+        <v>660</v>
       </c>
       <c r="F412" s="22"/>
       <c r="G412" s="23"/>
@@ -21406,14 +21573,14 @@
         <v>428</v>
       </c>
       <c r="B433" s="22"/>
-      <c r="C433" s="1" t="s">
+      <c r="C433" s="80" t="s">
         <v>580</v>
       </c>
-      <c r="D433" s="2">
-        <v>695</v>
-      </c>
-      <c r="E433" s="2">
-        <v>680</v>
+      <c r="D433" s="81">
+        <v>690</v>
+      </c>
+      <c r="E433" s="81">
+        <v>660</v>
       </c>
       <c r="F433" s="22"/>
       <c r="G433" s="23"/>
@@ -22833,7 +23000,7 @@
         <v>590</v>
       </c>
       <c r="E472" s="2">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="F472" s="22"/>
       <c r="G472" s="23"/>
@@ -23884,14 +24051,14 @@
         <v>496</v>
       </c>
       <c r="B501" s="22"/>
-      <c r="C501" s="1" t="s">
+      <c r="C501" s="82" t="s">
         <v>664</v>
       </c>
-      <c r="D501" s="2">
-        <v>640</v>
-      </c>
-      <c r="E501" s="2">
-        <v>635</v>
+      <c r="D501" s="83">
+        <v>680</v>
+      </c>
+      <c r="E501" s="83">
+        <v>665</v>
       </c>
       <c r="F501" s="1" t="s">
         <v>665</v>
@@ -24934,14 +25101,14 @@
         <v>524</v>
       </c>
       <c r="B529" s="22"/>
-      <c r="C529" s="1" t="s">
+      <c r="C529" s="80" t="s">
         <v>713</v>
       </c>
-      <c r="D529" s="2">
-        <v>625</v>
-      </c>
-      <c r="E529" s="2">
+      <c r="D529" s="81">
         <v>620</v>
+      </c>
+      <c r="E529" s="81">
+        <v>615</v>
       </c>
       <c r="F529" s="1" t="s">
         <v>714</v>
@@ -25190,14 +25357,14 @@
         <v>531</v>
       </c>
       <c r="B536" s="22"/>
-      <c r="C536" s="1" t="s">
+      <c r="C536" s="80" t="s">
         <v>722</v>
       </c>
-      <c r="D536" s="2">
-        <v>700</v>
-      </c>
-      <c r="E536" s="2">
-        <v>690</v>
+      <c r="D536" s="81">
+        <v>695</v>
+      </c>
+      <c r="E536" s="81">
+        <v>680</v>
       </c>
       <c r="F536" s="22"/>
       <c r="G536" s="23"/>
@@ -26002,14 +26169,14 @@
         <v>553</v>
       </c>
       <c r="B558" s="22"/>
-      <c r="C558" s="1" t="s">
+      <c r="C558" s="80" t="s">
         <v>754</v>
       </c>
-      <c r="D558" s="2">
-        <v>615</v>
-      </c>
-      <c r="E558" s="2">
-        <v>615</v>
+      <c r="D558" s="81">
+        <v>610</v>
+      </c>
+      <c r="E558" s="81">
+        <v>610</v>
       </c>
       <c r="F558" s="1" t="s">
         <v>755</v>
@@ -26114,13 +26281,13 @@
         <v>556</v>
       </c>
       <c r="B561" s="22"/>
-      <c r="C561" s="1" t="s">
+      <c r="C561" s="80" t="s">
         <v>759</v>
       </c>
-      <c r="D561" s="2">
-        <v>610</v>
-      </c>
-      <c r="E561" s="2">
+      <c r="D561" s="81">
+        <v>605</v>
+      </c>
+      <c r="E561" s="81">
         <v>605</v>
       </c>
       <c r="F561" s="22"/>
@@ -26296,14 +26463,14 @@
         <v>561</v>
       </c>
       <c r="B566" s="22"/>
-      <c r="C566" s="1" t="s">
+      <c r="C566" s="80" t="s">
         <v>765</v>
       </c>
-      <c r="D566" s="2">
-        <v>600</v>
-      </c>
-      <c r="E566" s="2">
-        <v>600</v>
+      <c r="D566" s="81">
+        <v>595</v>
+      </c>
+      <c r="E566" s="81">
+        <v>590</v>
       </c>
       <c r="F566" s="22"/>
       <c r="G566" s="23"/>
@@ -26374,7 +26541,7 @@
         <v>768</v>
       </c>
       <c r="D568" s="2">
-        <v>630</v>
+        <v>645</v>
       </c>
       <c r="E568" s="2">
         <v>625</v>
@@ -26708,14 +26875,14 @@
         <v>572</v>
       </c>
       <c r="B577" s="22"/>
-      <c r="C577" s="1" t="s">
+      <c r="C577" s="80" t="s">
         <v>784</v>
       </c>
-      <c r="D577" s="2">
-        <v>585</v>
-      </c>
-      <c r="E577" s="2">
-        <v>585</v>
+      <c r="D577" s="81">
+        <v>580</v>
+      </c>
+      <c r="E577" s="81">
+        <v>580</v>
       </c>
       <c r="F577" s="22"/>
       <c r="G577" s="20"/>
@@ -27932,13 +28099,13 @@
         <v>605</v>
       </c>
       <c r="B610" s="28"/>
-      <c r="C610" s="1" t="s">
+      <c r="C610" s="82" t="s">
         <v>834</v>
       </c>
-      <c r="D610" s="2">
-        <v>665</v>
-      </c>
-      <c r="E610" s="2">
+      <c r="D610" s="83">
+        <v>685</v>
+      </c>
+      <c r="E610" s="83">
         <v>655</v>
       </c>
       <c r="F610" s="1" t="s">
@@ -29936,14 +30103,14 @@
         <v>659</v>
       </c>
       <c r="B664" s="28"/>
-      <c r="C664" s="3" t="s">
+      <c r="C664" s="86" t="s">
         <v>918</v>
       </c>
-      <c r="D664" s="2">
-        <v>720</v>
-      </c>
-      <c r="E664" s="2">
-        <v>705</v>
+      <c r="D664" s="81">
+        <v>715</v>
+      </c>
+      <c r="E664" s="81">
+        <v>700</v>
       </c>
       <c r="F664" s="3" t="s">
         <v>919</v>
@@ -30376,13 +30543,13 @@
         <v>671</v>
       </c>
       <c r="B676" s="8"/>
-      <c r="C676" s="7" t="s">
+      <c r="C676" s="87" t="s">
         <v>1043</v>
       </c>
-      <c r="D676" s="2">
-        <v>645</v>
-      </c>
-      <c r="E676" s="2">
+      <c r="D676" s="83">
+        <v>655</v>
+      </c>
+      <c r="E676" s="83">
         <v>630</v>
       </c>
       <c r="F676" s="8"/>
@@ -30601,8 +30768,12 @@
       <c r="C682" s="8" t="s">
         <v>1072</v>
       </c>
-      <c r="D682" s="2"/>
-      <c r="E682" s="2"/>
+      <c r="D682" s="2">
+        <v>600</v>
+      </c>
+      <c r="E682" s="2">
+        <v>600</v>
+      </c>
       <c r="F682" s="40" t="s">
         <v>1073</v>
       </c>
@@ -31118,14 +31289,14 @@
         <v>691</v>
       </c>
       <c r="B696" s="8"/>
-      <c r="C696" s="8" t="s">
+      <c r="C696" s="88" t="s">
         <v>1095</v>
       </c>
-      <c r="D696" s="2">
-        <v>710</v>
-      </c>
-      <c r="E696" s="2">
-        <v>700</v>
+      <c r="D696" s="81">
+        <v>690</v>
+      </c>
+      <c r="E696" s="81">
+        <v>670</v>
       </c>
       <c r="F696" s="40" t="s">
         <v>1096</v>
@@ -31156,13 +31327,13 @@
         <v>692</v>
       </c>
       <c r="B697" s="8"/>
-      <c r="C697" s="8" t="s">
+      <c r="C697" s="88" t="s">
         <v>1097</v>
       </c>
-      <c r="D697" s="2">
-        <v>610</v>
-      </c>
-      <c r="E697" s="2">
+      <c r="D697" s="81">
+        <v>605</v>
+      </c>
+      <c r="E697" s="81">
         <v>600</v>
       </c>
       <c r="F697" s="40" t="s">
@@ -31349,7 +31520,7 @@
         <v>600</v>
       </c>
       <c r="E702" s="2">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="F702" s="28"/>
       <c r="G702" s="12"/>
@@ -31776,14 +31947,14 @@
         <v>709</v>
       </c>
       <c r="B714" s="8"/>
-      <c r="C714" s="8" t="s">
+      <c r="C714" s="89" t="s">
         <v>1116</v>
       </c>
-      <c r="D714" s="2">
+      <c r="D714" s="83">
+        <v>710</v>
+      </c>
+      <c r="E714" s="83">
         <v>680</v>
-      </c>
-      <c r="E714" s="2">
-        <v>670</v>
       </c>
       <c r="F714" s="28"/>
       <c r="G714" s="12"/>
@@ -31844,11 +32015,19 @@
       <c r="Z715" s="13"/>
     </row>
     <row r="716" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A716" s="12"/>
+      <c r="A716" s="8">
+        <v>711</v>
+      </c>
       <c r="B716" s="12"/>
-      <c r="C716" s="12"/>
-      <c r="D716" s="15"/>
-      <c r="E716" s="15"/>
+      <c r="C716" s="8" t="s">
+        <v>1237</v>
+      </c>
+      <c r="D716" s="38">
+        <v>790</v>
+      </c>
+      <c r="E716" s="38">
+        <v>770</v>
+      </c>
       <c r="F716" s="12"/>
       <c r="G716" s="12"/>
       <c r="H716" s="12"/>
@@ -31872,11 +32051,19 @@
       <c r="Z716" s="13"/>
     </row>
     <row r="717" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A717" s="12"/>
+      <c r="A717" s="8">
+        <v>712</v>
+      </c>
       <c r="B717" s="12"/>
-      <c r="C717" s="12"/>
-      <c r="D717" s="15"/>
-      <c r="E717" s="15"/>
+      <c r="C717" s="8" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D717" s="38">
+        <v>605</v>
+      </c>
+      <c r="E717" s="38">
+        <v>600</v>
+      </c>
       <c r="F717" s="12"/>
       <c r="G717" s="12"/>
       <c r="H717" s="12"/>
@@ -31900,11 +32087,19 @@
       <c r="Z717" s="13"/>
     </row>
     <row r="718" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A718" s="12"/>
+      <c r="A718" s="8">
+        <v>713</v>
+      </c>
       <c r="B718" s="12"/>
-      <c r="C718" s="12"/>
-      <c r="D718" s="15"/>
-      <c r="E718" s="15"/>
+      <c r="C718" s="8" t="s">
+        <v>1239</v>
+      </c>
+      <c r="D718" s="38">
+        <v>600</v>
+      </c>
+      <c r="E718" s="38">
+        <v>600</v>
+      </c>
       <c r="F718" s="12"/>
       <c r="G718" s="12"/>
       <c r="H718" s="12"/>
@@ -31928,11 +32123,19 @@
       <c r="Z718" s="13"/>
     </row>
     <row r="719" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A719" s="12"/>
+      <c r="A719" s="8">
+        <v>714</v>
+      </c>
       <c r="B719" s="12"/>
-      <c r="C719" s="12"/>
-      <c r="D719" s="15"/>
-      <c r="E719" s="15"/>
+      <c r="C719" s="8" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D719" s="38">
+        <v>635</v>
+      </c>
+      <c r="E719" s="38">
+        <v>620</v>
+      </c>
       <c r="F719" s="12"/>
       <c r="G719" s="12"/>
       <c r="H719" s="12"/>
@@ -31956,11 +32159,19 @@
       <c r="Z719" s="13"/>
     </row>
     <row r="720" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A720" s="12"/>
+      <c r="A720" s="8">
+        <v>715</v>
+      </c>
       <c r="B720" s="12"/>
-      <c r="C720" s="12"/>
-      <c r="D720" s="15"/>
-      <c r="E720" s="15"/>
+      <c r="C720" s="8" t="s">
+        <v>1241</v>
+      </c>
+      <c r="D720" s="38">
+        <v>635</v>
+      </c>
+      <c r="E720" s="38">
+        <v>615</v>
+      </c>
       <c r="F720" s="12"/>
       <c r="G720" s="12"/>
       <c r="H720" s="12"/>
@@ -31984,11 +32195,19 @@
       <c r="Z720" s="13"/>
     </row>
     <row r="721" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A721" s="12"/>
+      <c r="A721" s="8">
+        <v>716</v>
+      </c>
       <c r="B721" s="12"/>
-      <c r="C721" s="12"/>
-      <c r="D721" s="15"/>
-      <c r="E721" s="15"/>
+      <c r="C721" s="8" t="s">
+        <v>1242</v>
+      </c>
+      <c r="D721" s="38">
+        <v>610</v>
+      </c>
+      <c r="E721" s="38">
+        <v>600</v>
+      </c>
       <c r="F721" s="12"/>
       <c r="G721" s="12"/>
       <c r="H721" s="12"/>
@@ -32012,11 +32231,19 @@
       <c r="Z721" s="13"/>
     </row>
     <row r="722" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A722" s="12"/>
+      <c r="A722" s="8">
+        <v>717</v>
+      </c>
       <c r="B722" s="12"/>
-      <c r="C722" s="12"/>
-      <c r="D722" s="15"/>
-      <c r="E722" s="15"/>
+      <c r="C722" s="8" t="s">
+        <v>1243</v>
+      </c>
+      <c r="D722" s="38">
+        <v>610</v>
+      </c>
+      <c r="E722" s="38">
+        <v>600</v>
+      </c>
       <c r="F722" s="12"/>
       <c r="G722" s="12"/>
       <c r="H722" s="12"/>
@@ -32040,11 +32267,19 @@
       <c r="Z722" s="13"/>
     </row>
     <row r="723" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A723" s="12"/>
+      <c r="A723" s="8">
+        <v>718</v>
+      </c>
       <c r="B723" s="12"/>
-      <c r="C723" s="12"/>
-      <c r="D723" s="15"/>
-      <c r="E723" s="15"/>
+      <c r="C723" s="8" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D723" s="38">
+        <v>615</v>
+      </c>
+      <c r="E723" s="38">
+        <v>600</v>
+      </c>
       <c r="F723" s="12"/>
       <c r="G723" s="12"/>
       <c r="H723" s="12"/>
@@ -32068,11 +32303,19 @@
       <c r="Z723" s="13"/>
     </row>
     <row r="724" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A724" s="12"/>
+      <c r="A724" s="8">
+        <v>719</v>
+      </c>
       <c r="B724" s="12"/>
-      <c r="C724" s="12"/>
-      <c r="D724" s="15"/>
-      <c r="E724" s="15"/>
+      <c r="C724" s="8" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D724" s="38">
+        <v>615</v>
+      </c>
+      <c r="E724" s="38">
+        <v>600</v>
+      </c>
       <c r="F724" s="12"/>
       <c r="G724" s="12"/>
       <c r="H724" s="12"/>
@@ -32096,11 +32339,19 @@
       <c r="Z724" s="13"/>
     </row>
     <row r="725" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A725" s="12"/>
+      <c r="A725" s="8">
+        <v>720</v>
+      </c>
       <c r="B725" s="12"/>
-      <c r="C725" s="12"/>
-      <c r="D725" s="15"/>
-      <c r="E725" s="15"/>
+      <c r="C725" s="8" t="s">
+        <v>1246</v>
+      </c>
+      <c r="D725" s="38">
+        <v>610</v>
+      </c>
+      <c r="E725" s="38">
+        <v>600</v>
+      </c>
       <c r="F725" s="12"/>
       <c r="G725" s="12"/>
       <c r="H725" s="12"/>
@@ -32124,11 +32375,19 @@
       <c r="Z725" s="13"/>
     </row>
     <row r="726" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A726" s="12"/>
+      <c r="A726" s="8">
+        <v>721</v>
+      </c>
       <c r="B726" s="12"/>
-      <c r="C726" s="12"/>
-      <c r="D726" s="15"/>
-      <c r="E726" s="15"/>
+      <c r="C726" s="8" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D726" s="38">
+        <v>620</v>
+      </c>
+      <c r="E726" s="38">
+        <v>600</v>
+      </c>
       <c r="F726" s="12"/>
       <c r="G726" s="12"/>
       <c r="H726" s="12"/>
@@ -32152,11 +32411,19 @@
       <c r="Z726" s="13"/>
     </row>
     <row r="727" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A727" s="12"/>
+      <c r="A727" s="8">
+        <v>722</v>
+      </c>
       <c r="B727" s="12"/>
-      <c r="C727" s="12"/>
-      <c r="D727" s="15"/>
-      <c r="E727" s="15"/>
+      <c r="C727" s="8" t="s">
+        <v>1248</v>
+      </c>
+      <c r="D727" s="38">
+        <v>620</v>
+      </c>
+      <c r="E727" s="38">
+        <v>600</v>
+      </c>
       <c r="F727" s="12"/>
       <c r="G727" s="12"/>
       <c r="H727" s="12"/>
@@ -32180,11 +32447,19 @@
       <c r="Z727" s="13"/>
     </row>
     <row r="728" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A728" s="12"/>
+      <c r="A728" s="8">
+        <v>723</v>
+      </c>
       <c r="B728" s="12"/>
-      <c r="C728" s="12"/>
-      <c r="D728" s="15"/>
-      <c r="E728" s="15"/>
+      <c r="C728" s="8" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D728" s="38">
+        <v>630</v>
+      </c>
+      <c r="E728" s="38">
+        <v>615</v>
+      </c>
       <c r="F728" s="12"/>
       <c r="G728" s="12"/>
       <c r="H728" s="12"/>
@@ -32208,11 +32483,19 @@
       <c r="Z728" s="13"/>
     </row>
     <row r="729" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A729" s="12"/>
+      <c r="A729" s="8">
+        <v>724</v>
+      </c>
       <c r="B729" s="12"/>
-      <c r="C729" s="12"/>
-      <c r="D729" s="15"/>
-      <c r="E729" s="15"/>
+      <c r="C729" s="8" t="s">
+        <v>1250</v>
+      </c>
+      <c r="D729" s="38">
+        <v>635</v>
+      </c>
+      <c r="E729" s="38">
+        <v>615</v>
+      </c>
       <c r="F729" s="12"/>
       <c r="G729" s="12"/>
       <c r="H729" s="12"/>
@@ -32236,11 +32519,19 @@
       <c r="Z729" s="13"/>
     </row>
     <row r="730" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A730" s="12"/>
+      <c r="A730" s="8">
+        <v>725</v>
+      </c>
       <c r="B730" s="12"/>
-      <c r="C730" s="12"/>
-      <c r="D730" s="15"/>
-      <c r="E730" s="15"/>
+      <c r="C730" s="8" t="s">
+        <v>1251</v>
+      </c>
+      <c r="D730" s="38">
+        <v>620</v>
+      </c>
+      <c r="E730" s="38">
+        <v>610</v>
+      </c>
       <c r="F730" s="12"/>
       <c r="G730" s="12"/>
       <c r="H730" s="12"/>
@@ -32264,11 +32555,19 @@
       <c r="Z730" s="13"/>
     </row>
     <row r="731" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A731" s="12"/>
+      <c r="A731" s="8">
+        <v>726</v>
+      </c>
       <c r="B731" s="12"/>
-      <c r="C731" s="12"/>
-      <c r="D731" s="15"/>
-      <c r="E731" s="15"/>
+      <c r="C731" s="8" t="s">
+        <v>1252</v>
+      </c>
+      <c r="D731" s="38">
+        <v>640</v>
+      </c>
+      <c r="E731" s="38">
+        <v>620</v>
+      </c>
       <c r="F731" s="12"/>
       <c r="G731" s="12"/>
       <c r="H731" s="12"/>
@@ -32292,11 +32591,19 @@
       <c r="Z731" s="13"/>
     </row>
     <row r="732" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A732" s="12"/>
+      <c r="A732" s="8">
+        <v>727</v>
+      </c>
       <c r="B732" s="12"/>
-      <c r="C732" s="12"/>
-      <c r="D732" s="15"/>
-      <c r="E732" s="15"/>
+      <c r="C732" s="8" t="s">
+        <v>1253</v>
+      </c>
+      <c r="D732" s="38">
+        <v>610</v>
+      </c>
+      <c r="E732" s="38">
+        <v>600</v>
+      </c>
       <c r="F732" s="12"/>
       <c r="G732" s="12"/>
       <c r="H732" s="12"/>
@@ -32320,11 +32627,19 @@
       <c r="Z732" s="13"/>
     </row>
     <row r="733" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A733" s="12"/>
+      <c r="A733" s="8">
+        <v>728</v>
+      </c>
       <c r="B733" s="12"/>
-      <c r="C733" s="12"/>
-      <c r="D733" s="15"/>
-      <c r="E733" s="15"/>
+      <c r="C733" s="8" t="s">
+        <v>1254</v>
+      </c>
+      <c r="D733" s="38">
+        <v>610</v>
+      </c>
+      <c r="E733" s="38">
+        <v>605</v>
+      </c>
       <c r="F733" s="12"/>
       <c r="G733" s="12"/>
       <c r="H733" s="12"/>
@@ -32348,11 +32663,19 @@
       <c r="Z733" s="13"/>
     </row>
     <row r="734" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A734" s="12"/>
+      <c r="A734" s="8">
+        <v>729</v>
+      </c>
       <c r="B734" s="12"/>
-      <c r="C734" s="12"/>
-      <c r="D734" s="15"/>
-      <c r="E734" s="15"/>
+      <c r="C734" s="8" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D734" s="38">
+        <v>620</v>
+      </c>
+      <c r="E734" s="38">
+        <v>610</v>
+      </c>
       <c r="F734" s="12"/>
       <c r="G734" s="12"/>
       <c r="H734" s="12"/>
@@ -32376,11 +32699,19 @@
       <c r="Z734" s="13"/>
     </row>
     <row r="735" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A735" s="12"/>
+      <c r="A735" s="8">
+        <v>730</v>
+      </c>
       <c r="B735" s="12"/>
-      <c r="C735" s="12"/>
-      <c r="D735" s="15"/>
-      <c r="E735" s="15"/>
+      <c r="C735" s="8" t="s">
+        <v>1256</v>
+      </c>
+      <c r="D735" s="38">
+        <v>625</v>
+      </c>
+      <c r="E735" s="38">
+        <v>615</v>
+      </c>
       <c r="F735" s="12"/>
       <c r="G735" s="12"/>
       <c r="H735" s="12"/>
@@ -32404,11 +32735,19 @@
       <c r="Z735" s="13"/>
     </row>
     <row r="736" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A736" s="12"/>
+      <c r="A736" s="8">
+        <v>731</v>
+      </c>
       <c r="B736" s="12"/>
-      <c r="C736" s="12"/>
-      <c r="D736" s="15"/>
-      <c r="E736" s="15"/>
+      <c r="C736" s="88" t="s">
+        <v>1257</v>
+      </c>
+      <c r="D736" s="90">
+        <v>610</v>
+      </c>
+      <c r="E736" s="90">
+        <v>600</v>
+      </c>
       <c r="F736" s="12"/>
       <c r="G736" s="12"/>
       <c r="H736" s="12"/>
@@ -32432,11 +32771,19 @@
       <c r="Z736" s="13"/>
     </row>
     <row r="737" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A737" s="12"/>
+      <c r="A737" s="8">
+        <v>732</v>
+      </c>
       <c r="B737" s="12"/>
-      <c r="C737" s="12"/>
-      <c r="D737" s="15"/>
-      <c r="E737" s="15"/>
+      <c r="C737" s="88" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D737" s="90">
+        <v>630</v>
+      </c>
+      <c r="E737" s="90">
+        <v>615</v>
+      </c>
       <c r="F737" s="12"/>
       <c r="G737" s="12"/>
       <c r="H737" s="12"/>
@@ -32460,11 +32807,19 @@
       <c r="Z737" s="13"/>
     </row>
     <row r="738" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A738" s="12"/>
+      <c r="A738" s="8">
+        <v>733</v>
+      </c>
       <c r="B738" s="12"/>
-      <c r="C738" s="12"/>
-      <c r="D738" s="15"/>
-      <c r="E738" s="15"/>
+      <c r="C738" s="8" t="s">
+        <v>1259</v>
+      </c>
+      <c r="D738" s="38">
+        <v>600</v>
+      </c>
+      <c r="E738" s="38">
+        <v>600</v>
+      </c>
       <c r="F738" s="12"/>
       <c r="G738" s="12"/>
       <c r="H738" s="12"/>
@@ -32488,11 +32843,19 @@
       <c r="Z738" s="13"/>
     </row>
     <row r="739" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A739" s="12"/>
+      <c r="A739" s="8">
+        <v>734</v>
+      </c>
       <c r="B739" s="12"/>
-      <c r="C739" s="12"/>
-      <c r="D739" s="15"/>
-      <c r="E739" s="15"/>
+      <c r="C739" s="8" t="s">
+        <v>1260</v>
+      </c>
+      <c r="D739" s="38">
+        <v>600</v>
+      </c>
+      <c r="E739" s="38">
+        <v>600</v>
+      </c>
       <c r="F739" s="12"/>
       <c r="G739" s="12"/>
       <c r="H739" s="12"/>
@@ -32516,11 +32879,19 @@
       <c r="Z739" s="13"/>
     </row>
     <row r="740" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A740" s="12"/>
+      <c r="A740" s="8">
+        <v>735</v>
+      </c>
       <c r="B740" s="12"/>
-      <c r="C740" s="12"/>
-      <c r="D740" s="15"/>
-      <c r="E740" s="15"/>
+      <c r="C740" s="8" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D740" s="38">
+        <v>730</v>
+      </c>
+      <c r="E740" s="38">
+        <v>710</v>
+      </c>
       <c r="F740" s="12"/>
       <c r="G740" s="12"/>
       <c r="H740" s="12"/>
@@ -32544,11 +32915,19 @@
       <c r="Z740" s="13"/>
     </row>
     <row r="741" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A741" s="12"/>
+      <c r="A741" s="8">
+        <v>736</v>
+      </c>
       <c r="B741" s="12"/>
-      <c r="C741" s="12"/>
-      <c r="D741" s="15"/>
-      <c r="E741" s="15"/>
+      <c r="C741" s="8" t="s">
+        <v>1262</v>
+      </c>
+      <c r="D741" s="38">
+        <v>605</v>
+      </c>
+      <c r="E741" s="38">
+        <v>600</v>
+      </c>
       <c r="F741" s="12"/>
       <c r="G741" s="12"/>
       <c r="H741" s="12"/>
@@ -32572,11 +32951,19 @@
       <c r="Z741" s="13"/>
     </row>
     <row r="742" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A742" s="12"/>
+      <c r="A742" s="8">
+        <v>737</v>
+      </c>
       <c r="B742" s="12"/>
-      <c r="C742" s="12"/>
-      <c r="D742" s="15"/>
-      <c r="E742" s="15"/>
+      <c r="C742" s="8" t="s">
+        <v>1263</v>
+      </c>
+      <c r="D742" s="38">
+        <v>615</v>
+      </c>
+      <c r="E742" s="38">
+        <v>605</v>
+      </c>
       <c r="F742" s="12"/>
       <c r="G742" s="12"/>
       <c r="H742" s="12"/>
@@ -32600,11 +32987,19 @@
       <c r="Z742" s="13"/>
     </row>
     <row r="743" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A743" s="12"/>
+      <c r="A743" s="8">
+        <v>738</v>
+      </c>
       <c r="B743" s="12"/>
-      <c r="C743" s="12"/>
-      <c r="D743" s="15"/>
-      <c r="E743" s="15"/>
+      <c r="C743" s="8" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D743" s="38">
+        <v>625</v>
+      </c>
+      <c r="E743" s="38">
+        <v>620</v>
+      </c>
       <c r="F743" s="12"/>
       <c r="G743" s="12"/>
       <c r="H743" s="12"/>
@@ -32628,11 +33023,19 @@
       <c r="Z743" s="13"/>
     </row>
     <row r="744" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A744" s="12"/>
+      <c r="A744" s="8">
+        <v>739</v>
+      </c>
       <c r="B744" s="12"/>
-      <c r="C744" s="12"/>
-      <c r="D744" s="15"/>
-      <c r="E744" s="15"/>
+      <c r="C744" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D744" s="38">
+        <v>625</v>
+      </c>
+      <c r="E744" s="38">
+        <v>615</v>
+      </c>
       <c r="F744" s="12"/>
       <c r="G744" s="12"/>
       <c r="H744" s="12"/>
@@ -32656,11 +33059,19 @@
       <c r="Z744" s="13"/>
     </row>
     <row r="745" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A745" s="12"/>
+      <c r="A745" s="8">
+        <v>740</v>
+      </c>
       <c r="B745" s="12"/>
-      <c r="C745" s="12"/>
-      <c r="D745" s="15"/>
-      <c r="E745" s="15"/>
+      <c r="C745" s="8" t="s">
+        <v>1265</v>
+      </c>
+      <c r="D745" s="38">
+        <v>650</v>
+      </c>
+      <c r="E745" s="38">
+        <v>635</v>
+      </c>
       <c r="F745" s="12"/>
       <c r="G745" s="12"/>
       <c r="H745" s="12"/>
@@ -32684,11 +33095,19 @@
       <c r="Z745" s="13"/>
     </row>
     <row r="746" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A746" s="12"/>
+      <c r="A746" s="8">
+        <v>741</v>
+      </c>
       <c r="B746" s="12"/>
-      <c r="C746" s="12"/>
-      <c r="D746" s="15"/>
-      <c r="E746" s="15"/>
+      <c r="C746" s="8" t="s">
+        <v>1266</v>
+      </c>
+      <c r="D746" s="38">
+        <v>605</v>
+      </c>
+      <c r="E746" s="38">
+        <v>600</v>
+      </c>
       <c r="F746" s="12"/>
       <c r="G746" s="12"/>
       <c r="H746" s="12"/>
@@ -32712,11 +33131,19 @@
       <c r="Z746" s="13"/>
     </row>
     <row r="747" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A747" s="12"/>
+      <c r="A747" s="8">
+        <v>742</v>
+      </c>
       <c r="B747" s="12"/>
-      <c r="C747" s="12"/>
-      <c r="D747" s="15"/>
-      <c r="E747" s="15"/>
+      <c r="C747" s="8" t="s">
+        <v>1267</v>
+      </c>
+      <c r="D747" s="38">
+        <v>650</v>
+      </c>
+      <c r="E747" s="38">
+        <v>640</v>
+      </c>
       <c r="F747" s="12"/>
       <c r="G747" s="12"/>
       <c r="H747" s="12"/>
@@ -32740,11 +33167,19 @@
       <c r="Z747" s="13"/>
     </row>
     <row r="748" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A748" s="12"/>
+      <c r="A748" s="8">
+        <v>743</v>
+      </c>
       <c r="B748" s="12"/>
-      <c r="C748" s="12"/>
-      <c r="D748" s="15"/>
-      <c r="E748" s="15"/>
+      <c r="C748" s="8" t="s">
+        <v>1268</v>
+      </c>
+      <c r="D748" s="38">
+        <v>715</v>
+      </c>
+      <c r="E748" s="38">
+        <v>700</v>
+      </c>
       <c r="F748" s="12"/>
       <c r="G748" s="12"/>
       <c r="H748" s="12"/>
@@ -32768,11 +33203,19 @@
       <c r="Z748" s="13"/>
     </row>
     <row r="749" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A749" s="12"/>
+      <c r="A749" s="8">
+        <v>744</v>
+      </c>
       <c r="B749" s="12"/>
-      <c r="C749" s="12"/>
-      <c r="D749" s="15"/>
-      <c r="E749" s="15"/>
+      <c r="C749" s="8" t="s">
+        <v>1269</v>
+      </c>
+      <c r="D749" s="38">
+        <v>610</v>
+      </c>
+      <c r="E749" s="38">
+        <v>600</v>
+      </c>
       <c r="F749" s="12"/>
       <c r="G749" s="12"/>
       <c r="H749" s="12"/>
@@ -32796,11 +33239,19 @@
       <c r="Z749" s="13"/>
     </row>
     <row r="750" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A750" s="12"/>
+      <c r="A750" s="8">
+        <v>745</v>
+      </c>
       <c r="B750" s="12"/>
-      <c r="C750" s="12"/>
-      <c r="D750" s="15"/>
-      <c r="E750" s="15"/>
+      <c r="C750" s="8" t="s">
+        <v>1270</v>
+      </c>
+      <c r="D750" s="38">
+        <v>710</v>
+      </c>
+      <c r="E750" s="38">
+        <v>690</v>
+      </c>
       <c r="F750" s="12"/>
       <c r="G750" s="12"/>
       <c r="H750" s="12"/>
@@ -39841,8 +40292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -40522,13 +40973,13 @@
         <v>15</v>
       </c>
       <c r="B20" s="52"/>
-      <c r="C20" s="53" t="s">
+      <c r="C20" s="91" t="s">
         <v>1226</v>
       </c>
-      <c r="D20" s="2">
-        <v>610</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="81">
+        <v>605</v>
+      </c>
+      <c r="E20" s="81">
         <v>600</v>
       </c>
       <c r="F20" s="54" t="s">
@@ -40777,14 +41228,14 @@
         <v>22</v>
       </c>
       <c r="B27" s="52"/>
-      <c r="C27" s="53" t="s">
+      <c r="C27" s="91" t="s">
         <v>940</v>
       </c>
-      <c r="D27" s="2">
-        <v>640</v>
-      </c>
-      <c r="E27" s="2">
-        <v>630</v>
+      <c r="D27" s="81">
+        <v>625</v>
+      </c>
+      <c r="E27" s="81">
+        <v>610</v>
       </c>
       <c r="F27" s="55"/>
       <c r="G27" s="44"/>
@@ -41026,13 +41477,13 @@
         <v>29</v>
       </c>
       <c r="B34" s="55"/>
-      <c r="C34" s="54" t="s">
+      <c r="C34" s="92" t="s">
         <v>945</v>
       </c>
-      <c r="D34" s="2">
-        <v>660</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D34" s="81">
+        <v>655</v>
+      </c>
+      <c r="E34" s="81">
         <v>650</v>
       </c>
       <c r="F34" s="56"/>
@@ -41384,13 +41835,13 @@
         <v>39</v>
       </c>
       <c r="B44" s="56"/>
-      <c r="C44" s="54" t="s">
+      <c r="C44" s="93" t="s">
         <v>958</v>
       </c>
-      <c r="D44" s="2">
-        <v>640</v>
-      </c>
-      <c r="E44" s="2">
+      <c r="D44" s="83">
+        <v>655</v>
+      </c>
+      <c r="E44" s="83">
         <v>640</v>
       </c>
       <c r="F44" s="56"/>
@@ -41917,13 +42368,13 @@
         <v>54</v>
       </c>
       <c r="B59" s="56"/>
-      <c r="C59" s="54" t="s">
+      <c r="C59" s="93" t="s">
         <v>975</v>
       </c>
-      <c r="D59" s="2">
-        <v>630</v>
-      </c>
-      <c r="E59" s="2">
+      <c r="D59" s="83">
+        <v>635</v>
+      </c>
+      <c r="E59" s="83">
         <v>615</v>
       </c>
       <c r="F59" s="55"/>
@@ -42351,13 +42802,13 @@
         <v>66</v>
       </c>
       <c r="B71" s="56"/>
-      <c r="C71" s="54" t="s">
+      <c r="C71" s="93" t="s">
         <v>994</v>
       </c>
-      <c r="D71" s="2">
-        <v>620</v>
-      </c>
-      <c r="E71" s="2">
+      <c r="D71" s="83">
+        <v>625</v>
+      </c>
+      <c r="E71" s="83">
         <v>610</v>
       </c>
       <c r="F71" s="54" t="s">
@@ -42423,14 +42874,14 @@
         <v>68</v>
       </c>
       <c r="B73" s="56"/>
-      <c r="C73" s="54" t="s">
+      <c r="C73" s="92" t="s">
         <v>997</v>
       </c>
-      <c r="D73" s="2">
-        <v>650</v>
-      </c>
-      <c r="E73" s="2">
-        <v>640</v>
+      <c r="D73" s="81">
+        <v>645</v>
+      </c>
+      <c r="E73" s="81">
+        <v>635</v>
       </c>
       <c r="F73" s="55"/>
       <c r="G73" s="44"/>
@@ -42458,13 +42909,13 @@
         <v>69</v>
       </c>
       <c r="B74" s="55"/>
-      <c r="C74" s="54" t="s">
+      <c r="C74" s="93" t="s">
         <v>998</v>
       </c>
-      <c r="D74" s="2">
-        <v>615</v>
-      </c>
-      <c r="E74" s="2">
+      <c r="D74" s="83">
+        <v>620</v>
+      </c>
+      <c r="E74" s="83">
         <v>600</v>
       </c>
       <c r="F74" s="55"/>
@@ -42672,13 +43123,13 @@
         <v>75</v>
       </c>
       <c r="B80" s="55"/>
-      <c r="C80" s="54" t="s">
+      <c r="C80" s="92" t="s">
         <v>1006</v>
       </c>
-      <c r="D80" s="2">
-        <v>660</v>
-      </c>
-      <c r="E80" s="2">
+      <c r="D80" s="81">
+        <v>655</v>
+      </c>
+      <c r="E80" s="81">
         <v>640</v>
       </c>
       <c r="F80" s="55"/>
@@ -43575,13 +44026,13 @@
         <v>100</v>
       </c>
       <c r="B105" s="8"/>
-      <c r="C105" s="8" t="s">
+      <c r="C105" s="88" t="s">
         <v>1071</v>
       </c>
-      <c r="D105" s="2">
+      <c r="D105" s="81">
         <v>560</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105" s="81">
         <v>560</v>
       </c>
       <c r="F105" s="8"/>
@@ -43606,11 +44057,19 @@
       <c r="Y105" s="56"/>
     </row>
     <row r="106" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="44"/>
+      <c r="A106" s="44">
+        <v>101</v>
+      </c>
       <c r="B106" s="44"/>
-      <c r="C106" s="44"/>
-      <c r="D106" s="47"/>
-      <c r="E106" s="47"/>
+      <c r="C106" s="8" t="s">
+        <v>1271</v>
+      </c>
+      <c r="D106" s="38">
+        <v>590</v>
+      </c>
+      <c r="E106" s="38">
+        <v>580</v>
+      </c>
       <c r="F106" s="44"/>
       <c r="G106" s="44"/>
       <c r="H106" s="44"/>

</xml_diff>

<commit_message>
chore: update bao vung tau
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C453FD8-2AD6-3D4B-9824-27FB90962250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88899278-B9B9-BE4A-BABD-A8F9030B9B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3580" yWindow="760" windowWidth="27860" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="1314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="1315">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -3976,6 +3976,9 @@
   </si>
   <si>
     <t>Ngân Tiền Giang</t>
+  </si>
+  <si>
+    <t>Bảo Vũng Tàu</t>
   </si>
 </sst>
 </file>
@@ -4652,23 +4655,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4689,6 +4675,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5893,8 +5896,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E748" sqref="E748"/>
+      <pane ySplit="4" topLeftCell="A717" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J752" sqref="J752"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5902,7 +5905,7 @@
     <col min="1" max="1" width="7.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
-    <col min="4" max="5" width="16.5" style="149" customWidth="1"/>
+    <col min="4" max="5" width="16.5" style="142" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" style="2" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" customWidth="1"/>
@@ -5913,17 +5916,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="141" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
-      <c r="I1" s="142"/>
+      <c r="A1" s="152" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="153"/>
+      <c r="C1" s="153"/>
+      <c r="D1" s="153"/>
+      <c r="E1" s="153"/>
+      <c r="F1" s="153"/>
+      <c r="G1" s="153"/>
+      <c r="H1" s="153"/>
+      <c r="I1" s="153"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -5942,17 +5945,17 @@
       <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="141" t="s">
+      <c r="A2" s="152" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
-      <c r="I2" s="142"/>
+      <c r="B2" s="153"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="153"/>
+      <c r="E2" s="153"/>
+      <c r="F2" s="153"/>
+      <c r="G2" s="153"/>
+      <c r="H2" s="153"/>
+      <c r="I2" s="153"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -6007,10 +6010,10 @@
       <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="143" t="s">
+      <c r="D4" s="154" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="144"/>
+      <c r="E4" s="155"/>
       <c r="F4" s="5" t="s">
         <v>6</v>
       </c>
@@ -34239,20 +34242,20 @@
       <c r="Y610" s="61"/>
     </row>
     <row r="611" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A611" s="150">
+      <c r="A611" s="143">
         <v>606</v>
       </c>
-      <c r="B611" s="151"/>
-      <c r="C611" s="152" t="s">
+      <c r="B611" s="144"/>
+      <c r="C611" s="145" t="s">
         <v>878</v>
       </c>
-      <c r="D611" s="153">
+      <c r="D611" s="146">
         <v>605</v>
       </c>
-      <c r="E611" s="153">
+      <c r="E611" s="146">
         <v>600</v>
       </c>
-      <c r="F611" s="154" t="s">
+      <c r="F611" s="147" t="s">
         <v>879</v>
       </c>
       <c r="G611" s="1"/>
@@ -36871,8 +36874,8 @@
       <c r="A668" s="11">
         <v>663</v>
       </c>
-      <c r="B668" s="155"/>
-      <c r="C668" s="155" t="s">
+      <c r="B668" s="148"/>
+      <c r="C668" s="148" t="s">
         <v>1083</v>
       </c>
       <c r="D668" s="13">
@@ -37186,8 +37189,8 @@
       <c r="A675" s="11">
         <v>670</v>
       </c>
-      <c r="B675" s="156"/>
-      <c r="C675" s="157" t="s">
+      <c r="B675" s="149"/>
+      <c r="C675" s="150" t="s">
         <v>1090</v>
       </c>
       <c r="D675" s="13">
@@ -37232,7 +37235,7 @@
         <v>671</v>
       </c>
       <c r="B676" s="61"/>
-      <c r="C676" s="158" t="s">
+      <c r="C676" s="151" t="s">
         <v>1091</v>
       </c>
       <c r="D676" s="58">
@@ -40713,11 +40716,19 @@
       <c r="Y752" s="1"/>
     </row>
     <row r="753" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A753" s="4"/>
+      <c r="A753" s="4">
+        <v>748</v>
+      </c>
       <c r="B753" s="4"/>
-      <c r="C753" s="4"/>
-      <c r="D753" s="105"/>
-      <c r="E753" s="105"/>
+      <c r="C753" s="4" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D753" s="105">
+        <v>725</v>
+      </c>
+      <c r="E753" s="105">
+        <v>710</v>
+      </c>
       <c r="F753" s="17"/>
       <c r="G753" s="1"/>
       <c r="H753" s="1"/>
@@ -47385,8 +47396,8 @@
       <c r="A1000" s="1"/>
       <c r="B1000" s="1"/>
       <c r="C1000" s="1"/>
-      <c r="D1000" s="148"/>
-      <c r="E1000" s="148"/>
+      <c r="D1000" s="141"/>
+      <c r="E1000" s="141"/>
       <c r="F1000" s="1"/>
       <c r="G1000" s="1"/>
       <c r="H1000" s="1"/>
@@ -47458,17 +47469,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="145" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="146"/>
-      <c r="C1" s="146"/>
-      <c r="D1" s="146"/>
-      <c r="E1" s="146"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="146"/>
-      <c r="H1" s="146"/>
-      <c r="I1" s="146"/>
+      <c r="A1" s="156" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="157"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
       <c r="L1" s="32"/>
@@ -47488,17 +47499,17 @@
       <c r="Z1" s="32"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="156" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="146"/>
-      <c r="C2" s="146"/>
-      <c r="D2" s="146"/>
-      <c r="E2" s="146"/>
-      <c r="F2" s="146"/>
-      <c r="G2" s="146"/>
-      <c r="H2" s="146"/>
-      <c r="I2" s="146"/>
+      <c r="B2" s="157"/>
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="157"/>
+      <c r="I2" s="157"/>
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
       <c r="L2" s="32"/>
@@ -47555,10 +47566,10 @@
       <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="145" t="s">
+      <c r="D4" s="156" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="147"/>
+      <c r="E4" s="158"/>
       <c r="F4" s="31" t="s">
         <v>6</v>
       </c>
@@ -47574,10 +47585,10 @@
       <c r="J4" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="145" t="s">
+      <c r="K4" s="156" t="s">
         <v>1074</v>
       </c>
-      <c r="L4" s="147"/>
+      <c r="L4" s="158"/>
       <c r="M4" s="37" t="s">
         <v>1075</v>
       </c>

</xml_diff>

<commit_message>
score: update jun 1
</commit_message>
<xml_diff>
--- a/pages/api/score/data.xlsx
+++ b/pages/api/score/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daiduong.nguyen/node/dflyapp/tennis-btn/pages/api/score/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D624E26-B530-F547-9C09-66E6DC26CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9D2548-93B4-044C-9EEE-800413EA0CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="760" windowWidth="27860" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="1318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="1321">
   <si>
     <t>BẢNG ĐIỂM DIỄN ĐÀN TENNIS BẮC TRUNG NAM</t>
   </si>
@@ -3988,6 +3988,15 @@
   </si>
   <si>
     <t>Hùng RMit</t>
+  </si>
+  <si>
+    <t>Tòng Trung Thiện</t>
+  </si>
+  <si>
+    <t>Phạm Thành</t>
+  </si>
+  <si>
+    <t>0765025484</t>
   </si>
 </sst>
 </file>
@@ -4705,7 +4714,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -4713,6 +4722,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5905,8 +5924,8 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A652" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C675" sqref="C675"/>
+      <pane ySplit="4" topLeftCell="A713" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F759" sqref="F759"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29410,10 +29429,10 @@
         <v>708</v>
       </c>
       <c r="D506" s="13">
+        <v>680</v>
+      </c>
+      <c r="E506" s="13">
         <v>660</v>
-      </c>
-      <c r="E506" s="13">
-        <v>655</v>
       </c>
       <c r="F506" s="21" t="s">
         <v>709</v>
@@ -29429,11 +29448,11 @@
       </c>
       <c r="L506" s="14">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M506" s="14">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N506" s="1"/>
       <c r="O506" s="1"/>
@@ -40780,10 +40799,10 @@
         <v>1311</v>
       </c>
       <c r="D754" s="105">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="E754" s="105">
-        <v>690</v>
+        <v>675</v>
       </c>
       <c r="F754" s="17"/>
       <c r="G754" s="1"/>
@@ -40797,11 +40816,11 @@
       </c>
       <c r="L754" s="116">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="M754" s="116">
         <f t="shared" si="29"/>
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="N754" s="1"/>
       <c r="O754" s="1"/>
@@ -40886,11 +40905,11 @@
         <v>610</v>
       </c>
       <c r="L756" s="116">
-        <f t="shared" ref="L756:L757" si="30">D756-J756</f>
+        <f t="shared" ref="L756:L758" si="30">D756-J756</f>
         <v>0</v>
       </c>
       <c r="M756" s="116">
-        <f t="shared" ref="M756:M757" si="31">E756-K756</f>
+        <f t="shared" ref="M756:M758" si="31">E756-K756</f>
         <v>0</v>
       </c>
       <c r="N756" s="1"/>
@@ -40952,19 +40971,39 @@
       <c r="Y757" s="1"/>
     </row>
     <row r="758" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A758" s="4"/>
+      <c r="A758" s="4">
+        <v>753</v>
+      </c>
       <c r="B758" s="4"/>
-      <c r="C758" s="4"/>
-      <c r="D758" s="105"/>
-      <c r="E758" s="105"/>
-      <c r="F758" s="17"/>
+      <c r="C758" s="4" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D758" s="105">
+        <v>740</v>
+      </c>
+      <c r="E758" s="105">
+        <v>720</v>
+      </c>
+      <c r="F758" s="103" t="s">
+        <v>1320</v>
+      </c>
       <c r="G758" s="1"/>
       <c r="H758" s="1"/>
       <c r="I758" s="1"/>
-      <c r="J758" s="1"/>
-      <c r="K758" s="1"/>
-      <c r="L758" s="1"/>
-      <c r="M758" s="1"/>
+      <c r="J758" s="1">
+        <v>740</v>
+      </c>
+      <c r="K758" s="1">
+        <v>720</v>
+      </c>
+      <c r="L758" s="1">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="M758" s="1">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
       <c r="N758" s="1"/>
       <c r="O758" s="1"/>
       <c r="P758" s="1"/>
@@ -40979,11 +41018,19 @@
       <c r="Y758" s="1"/>
     </row>
     <row r="759" spans="1:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A759" s="4"/>
+      <c r="A759" s="4">
+        <v>754</v>
+      </c>
       <c r="B759" s="4"/>
-      <c r="C759" s="4"/>
-      <c r="D759" s="105"/>
-      <c r="E759" s="105"/>
+      <c r="C759" s="4" t="s">
+        <v>1319</v>
+      </c>
+      <c r="D759" s="105">
+        <v>605</v>
+      </c>
+      <c r="E759" s="105">
+        <v>600</v>
+      </c>
       <c r="F759" s="17"/>
       <c r="G759" s="1"/>
       <c r="H759" s="1"/>
@@ -47520,12 +47567,15 @@
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="L1:M3 M4 L5:M1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>